<commit_message>
Updates for December 2013
</commit_message>
<xml_diff>
--- a/dataPackages/dataPackagesInDryad.xlsx
+++ b/dataPackages/dataPackagesInDryad.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="17740" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="17740" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="SubmissionDates" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -139,10 +138,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>SubmissionDates!$A$1:$A$4324</c:f>
+              <c:f>SubmissionDates!$A$1:$A$4524</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="4324"/>
+                <c:ptCount val="4524"/>
                 <c:pt idx="0">
                   <c:v>39422.0</c:v>
                 </c:pt>
@@ -13114,16 +13113,616 @@
                 </c:pt>
                 <c:pt idx="4323">
                   <c:v>41597.0</c:v>
+                </c:pt>
+                <c:pt idx="4324">
+                  <c:v>41597.0</c:v>
+                </c:pt>
+                <c:pt idx="4325">
+                  <c:v>41597.0</c:v>
+                </c:pt>
+                <c:pt idx="4326">
+                  <c:v>41598.0</c:v>
+                </c:pt>
+                <c:pt idx="4327">
+                  <c:v>41598.0</c:v>
+                </c:pt>
+                <c:pt idx="4328">
+                  <c:v>41598.0</c:v>
+                </c:pt>
+                <c:pt idx="4329">
+                  <c:v>41598.0</c:v>
+                </c:pt>
+                <c:pt idx="4330">
+                  <c:v>41598.0</c:v>
+                </c:pt>
+                <c:pt idx="4331">
+                  <c:v>41599.0</c:v>
+                </c:pt>
+                <c:pt idx="4332">
+                  <c:v>41599.0</c:v>
+                </c:pt>
+                <c:pt idx="4333">
+                  <c:v>41599.0</c:v>
+                </c:pt>
+                <c:pt idx="4334">
+                  <c:v>41599.0</c:v>
+                </c:pt>
+                <c:pt idx="4335">
+                  <c:v>41599.0</c:v>
+                </c:pt>
+                <c:pt idx="4336">
+                  <c:v>41599.0</c:v>
+                </c:pt>
+                <c:pt idx="4337">
+                  <c:v>41599.0</c:v>
+                </c:pt>
+                <c:pt idx="4338">
+                  <c:v>41599.0</c:v>
+                </c:pt>
+                <c:pt idx="4339">
+                  <c:v>41603.0</c:v>
+                </c:pt>
+                <c:pt idx="4340">
+                  <c:v>41603.0</c:v>
+                </c:pt>
+                <c:pt idx="4341">
+                  <c:v>41603.0</c:v>
+                </c:pt>
+                <c:pt idx="4342">
+                  <c:v>41603.0</c:v>
+                </c:pt>
+                <c:pt idx="4343">
+                  <c:v>41603.0</c:v>
+                </c:pt>
+                <c:pt idx="4344">
+                  <c:v>41604.0</c:v>
+                </c:pt>
+                <c:pt idx="4345">
+                  <c:v>41604.0</c:v>
+                </c:pt>
+                <c:pt idx="4346">
+                  <c:v>41604.0</c:v>
+                </c:pt>
+                <c:pt idx="4347">
+                  <c:v>41604.0</c:v>
+                </c:pt>
+                <c:pt idx="4348">
+                  <c:v>41604.0</c:v>
+                </c:pt>
+                <c:pt idx="4349">
+                  <c:v>41604.0</c:v>
+                </c:pt>
+                <c:pt idx="4350">
+                  <c:v>41605.0</c:v>
+                </c:pt>
+                <c:pt idx="4351">
+                  <c:v>41605.0</c:v>
+                </c:pt>
+                <c:pt idx="4352">
+                  <c:v>41605.0</c:v>
+                </c:pt>
+                <c:pt idx="4353">
+                  <c:v>41605.0</c:v>
+                </c:pt>
+                <c:pt idx="4354">
+                  <c:v>41605.0</c:v>
+                </c:pt>
+                <c:pt idx="4355">
+                  <c:v>41605.0</c:v>
+                </c:pt>
+                <c:pt idx="4356">
+                  <c:v>41605.0</c:v>
+                </c:pt>
+                <c:pt idx="4357">
+                  <c:v>41605.0</c:v>
+                </c:pt>
+                <c:pt idx="4358">
+                  <c:v>41607.0</c:v>
+                </c:pt>
+                <c:pt idx="4359">
+                  <c:v>41607.0</c:v>
+                </c:pt>
+                <c:pt idx="4360">
+                  <c:v>41607.0</c:v>
+                </c:pt>
+                <c:pt idx="4361">
+                  <c:v>41610.0</c:v>
+                </c:pt>
+                <c:pt idx="4362">
+                  <c:v>41610.0</c:v>
+                </c:pt>
+                <c:pt idx="4363">
+                  <c:v>41610.0</c:v>
+                </c:pt>
+                <c:pt idx="4364">
+                  <c:v>41610.0</c:v>
+                </c:pt>
+                <c:pt idx="4365">
+                  <c:v>41611.0</c:v>
+                </c:pt>
+                <c:pt idx="4366">
+                  <c:v>41611.0</c:v>
+                </c:pt>
+                <c:pt idx="4367">
+                  <c:v>41611.0</c:v>
+                </c:pt>
+                <c:pt idx="4368">
+                  <c:v>41611.0</c:v>
+                </c:pt>
+                <c:pt idx="4369">
+                  <c:v>41611.0</c:v>
+                </c:pt>
+                <c:pt idx="4370">
+                  <c:v>41611.0</c:v>
+                </c:pt>
+                <c:pt idx="4371">
+                  <c:v>41611.0</c:v>
+                </c:pt>
+                <c:pt idx="4372">
+                  <c:v>41611.0</c:v>
+                </c:pt>
+                <c:pt idx="4373">
+                  <c:v>41611.0</c:v>
+                </c:pt>
+                <c:pt idx="4374">
+                  <c:v>41612.0</c:v>
+                </c:pt>
+                <c:pt idx="4375">
+                  <c:v>41612.0</c:v>
+                </c:pt>
+                <c:pt idx="4376">
+                  <c:v>41612.0</c:v>
+                </c:pt>
+                <c:pt idx="4377">
+                  <c:v>41612.0</c:v>
+                </c:pt>
+                <c:pt idx="4378">
+                  <c:v>41613.0</c:v>
+                </c:pt>
+                <c:pt idx="4379">
+                  <c:v>41613.0</c:v>
+                </c:pt>
+                <c:pt idx="4380">
+                  <c:v>41613.0</c:v>
+                </c:pt>
+                <c:pt idx="4381">
+                  <c:v>41613.0</c:v>
+                </c:pt>
+                <c:pt idx="4382">
+                  <c:v>41613.0</c:v>
+                </c:pt>
+                <c:pt idx="4383">
+                  <c:v>41613.0</c:v>
+                </c:pt>
+                <c:pt idx="4384">
+                  <c:v>41613.0</c:v>
+                </c:pt>
+                <c:pt idx="4385">
+                  <c:v>41613.0</c:v>
+                </c:pt>
+                <c:pt idx="4386">
+                  <c:v>41613.0</c:v>
+                </c:pt>
+                <c:pt idx="4387">
+                  <c:v>41613.0</c:v>
+                </c:pt>
+                <c:pt idx="4388">
+                  <c:v>41613.0</c:v>
+                </c:pt>
+                <c:pt idx="4389">
+                  <c:v>41613.0</c:v>
+                </c:pt>
+                <c:pt idx="4390">
+                  <c:v>41613.0</c:v>
+                </c:pt>
+                <c:pt idx="4391">
+                  <c:v>41613.0</c:v>
+                </c:pt>
+                <c:pt idx="4392">
+                  <c:v>41613.0</c:v>
+                </c:pt>
+                <c:pt idx="4393">
+                  <c:v>41614.0</c:v>
+                </c:pt>
+                <c:pt idx="4394">
+                  <c:v>41614.0</c:v>
+                </c:pt>
+                <c:pt idx="4395">
+                  <c:v>41617.0</c:v>
+                </c:pt>
+                <c:pt idx="4396">
+                  <c:v>41617.0</c:v>
+                </c:pt>
+                <c:pt idx="4397">
+                  <c:v>41617.0</c:v>
+                </c:pt>
+                <c:pt idx="4398">
+                  <c:v>41617.0</c:v>
+                </c:pt>
+                <c:pt idx="4399">
+                  <c:v>41617.0</c:v>
+                </c:pt>
+                <c:pt idx="4400">
+                  <c:v>41617.0</c:v>
+                </c:pt>
+                <c:pt idx="4401">
+                  <c:v>41617.0</c:v>
+                </c:pt>
+                <c:pt idx="4402">
+                  <c:v>41617.0</c:v>
+                </c:pt>
+                <c:pt idx="4403">
+                  <c:v>41617.0</c:v>
+                </c:pt>
+                <c:pt idx="4404">
+                  <c:v>41617.0</c:v>
+                </c:pt>
+                <c:pt idx="4405">
+                  <c:v>41617.0</c:v>
+                </c:pt>
+                <c:pt idx="4406">
+                  <c:v>41617.0</c:v>
+                </c:pt>
+                <c:pt idx="4407">
+                  <c:v>41617.0</c:v>
+                </c:pt>
+                <c:pt idx="4408">
+                  <c:v>41617.0</c:v>
+                </c:pt>
+                <c:pt idx="4409">
+                  <c:v>41617.0</c:v>
+                </c:pt>
+                <c:pt idx="4410">
+                  <c:v>41617.0</c:v>
+                </c:pt>
+                <c:pt idx="4411">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4412">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4413">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4414">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4415">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4416">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4417">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4418">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4419">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4420">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4421">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4422">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4423">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4424">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4425">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4426">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4427">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4428">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4429">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4430">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4431">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4432">
+                  <c:v>41618.0</c:v>
+                </c:pt>
+                <c:pt idx="4433">
+                  <c:v>41619.0</c:v>
+                </c:pt>
+                <c:pt idx="4434">
+                  <c:v>41619.0</c:v>
+                </c:pt>
+                <c:pt idx="4435">
+                  <c:v>41619.0</c:v>
+                </c:pt>
+                <c:pt idx="4436">
+                  <c:v>41619.0</c:v>
+                </c:pt>
+                <c:pt idx="4437">
+                  <c:v>41619.0</c:v>
+                </c:pt>
+                <c:pt idx="4438">
+                  <c:v>41619.0</c:v>
+                </c:pt>
+                <c:pt idx="4439">
+                  <c:v>41619.0</c:v>
+                </c:pt>
+                <c:pt idx="4440">
+                  <c:v>41619.0</c:v>
+                </c:pt>
+                <c:pt idx="4441">
+                  <c:v>41620.0</c:v>
+                </c:pt>
+                <c:pt idx="4442">
+                  <c:v>41620.0</c:v>
+                </c:pt>
+                <c:pt idx="4443">
+                  <c:v>41620.0</c:v>
+                </c:pt>
+                <c:pt idx="4444">
+                  <c:v>41620.0</c:v>
+                </c:pt>
+                <c:pt idx="4445">
+                  <c:v>41620.0</c:v>
+                </c:pt>
+                <c:pt idx="4446">
+                  <c:v>41621.0</c:v>
+                </c:pt>
+                <c:pt idx="4447">
+                  <c:v>41621.0</c:v>
+                </c:pt>
+                <c:pt idx="4448">
+                  <c:v>41621.0</c:v>
+                </c:pt>
+                <c:pt idx="4449">
+                  <c:v>41621.0</c:v>
+                </c:pt>
+                <c:pt idx="4450">
+                  <c:v>41621.0</c:v>
+                </c:pt>
+                <c:pt idx="4451">
+                  <c:v>41621.0</c:v>
+                </c:pt>
+                <c:pt idx="4452">
+                  <c:v>41621.0</c:v>
+                </c:pt>
+                <c:pt idx="4453">
+                  <c:v>41621.0</c:v>
+                </c:pt>
+                <c:pt idx="4454">
+                  <c:v>41625.0</c:v>
+                </c:pt>
+                <c:pt idx="4455">
+                  <c:v>41625.0</c:v>
+                </c:pt>
+                <c:pt idx="4456">
+                  <c:v>41625.0</c:v>
+                </c:pt>
+                <c:pt idx="4457">
+                  <c:v>41625.0</c:v>
+                </c:pt>
+                <c:pt idx="4458">
+                  <c:v>41625.0</c:v>
+                </c:pt>
+                <c:pt idx="4459">
+                  <c:v>41625.0</c:v>
+                </c:pt>
+                <c:pt idx="4460">
+                  <c:v>41625.0</c:v>
+                </c:pt>
+                <c:pt idx="4461">
+                  <c:v>41625.0</c:v>
+                </c:pt>
+                <c:pt idx="4462">
+                  <c:v>41625.0</c:v>
+                </c:pt>
+                <c:pt idx="4463">
+                  <c:v>41625.0</c:v>
+                </c:pt>
+                <c:pt idx="4464">
+                  <c:v>41625.0</c:v>
+                </c:pt>
+                <c:pt idx="4465">
+                  <c:v>41625.0</c:v>
+                </c:pt>
+                <c:pt idx="4466">
+                  <c:v>41626.0</c:v>
+                </c:pt>
+                <c:pt idx="4467">
+                  <c:v>41626.0</c:v>
+                </c:pt>
+                <c:pt idx="4468">
+                  <c:v>41626.0</c:v>
+                </c:pt>
+                <c:pt idx="4469">
+                  <c:v>41626.0</c:v>
+                </c:pt>
+                <c:pt idx="4470">
+                  <c:v>41626.0</c:v>
+                </c:pt>
+                <c:pt idx="4471">
+                  <c:v>41626.0</c:v>
+                </c:pt>
+                <c:pt idx="4472">
+                  <c:v>41626.0</c:v>
+                </c:pt>
+                <c:pt idx="4473">
+                  <c:v>41627.0</c:v>
+                </c:pt>
+                <c:pt idx="4474">
+                  <c:v>41627.0</c:v>
+                </c:pt>
+                <c:pt idx="4475">
+                  <c:v>41627.0</c:v>
+                </c:pt>
+                <c:pt idx="4476">
+                  <c:v>41627.0</c:v>
+                </c:pt>
+                <c:pt idx="4477">
+                  <c:v>41628.0</c:v>
+                </c:pt>
+                <c:pt idx="4478">
+                  <c:v>41628.0</c:v>
+                </c:pt>
+                <c:pt idx="4479">
+                  <c:v>41628.0</c:v>
+                </c:pt>
+                <c:pt idx="4480">
+                  <c:v>41628.0</c:v>
+                </c:pt>
+                <c:pt idx="4481">
+                  <c:v>41628.0</c:v>
+                </c:pt>
+                <c:pt idx="4482">
+                  <c:v>41628.0</c:v>
+                </c:pt>
+                <c:pt idx="4483">
+                  <c:v>41628.0</c:v>
+                </c:pt>
+                <c:pt idx="4484">
+                  <c:v>41631.0</c:v>
+                </c:pt>
+                <c:pt idx="4485">
+                  <c:v>41631.0</c:v>
+                </c:pt>
+                <c:pt idx="4486">
+                  <c:v>41631.0</c:v>
+                </c:pt>
+                <c:pt idx="4487">
+                  <c:v>41635.0</c:v>
+                </c:pt>
+                <c:pt idx="4488">
+                  <c:v>41635.0</c:v>
+                </c:pt>
+                <c:pt idx="4489">
+                  <c:v>41635.0</c:v>
+                </c:pt>
+                <c:pt idx="4490">
+                  <c:v>41635.0</c:v>
+                </c:pt>
+                <c:pt idx="4491">
+                  <c:v>41635.0</c:v>
+                </c:pt>
+                <c:pt idx="4492">
+                  <c:v>41638.0</c:v>
+                </c:pt>
+                <c:pt idx="4493">
+                  <c:v>41640.0</c:v>
+                </c:pt>
+                <c:pt idx="4494">
+                  <c:v>41641.0</c:v>
+                </c:pt>
+                <c:pt idx="4495">
+                  <c:v>41641.0</c:v>
+                </c:pt>
+                <c:pt idx="4496">
+                  <c:v>41641.0</c:v>
+                </c:pt>
+                <c:pt idx="4497">
+                  <c:v>41641.0</c:v>
+                </c:pt>
+                <c:pt idx="4498">
+                  <c:v>41641.0</c:v>
+                </c:pt>
+                <c:pt idx="4499">
+                  <c:v>41641.0</c:v>
+                </c:pt>
+                <c:pt idx="4500">
+                  <c:v>41641.0</c:v>
+                </c:pt>
+                <c:pt idx="4501">
+                  <c:v>41641.0</c:v>
+                </c:pt>
+                <c:pt idx="4502">
+                  <c:v>41641.0</c:v>
+                </c:pt>
+                <c:pt idx="4503">
+                  <c:v>41641.0</c:v>
+                </c:pt>
+                <c:pt idx="4504">
+                  <c:v>41641.0</c:v>
+                </c:pt>
+                <c:pt idx="4505">
+                  <c:v>41641.0</c:v>
+                </c:pt>
+                <c:pt idx="4506">
+                  <c:v>41642.0</c:v>
+                </c:pt>
+                <c:pt idx="4507">
+                  <c:v>41642.0</c:v>
+                </c:pt>
+                <c:pt idx="4508">
+                  <c:v>41642.0</c:v>
+                </c:pt>
+                <c:pt idx="4509">
+                  <c:v>41642.0</c:v>
+                </c:pt>
+                <c:pt idx="4510">
+                  <c:v>41642.0</c:v>
+                </c:pt>
+                <c:pt idx="4511">
+                  <c:v>41645.0</c:v>
+                </c:pt>
+                <c:pt idx="4512">
+                  <c:v>41645.0</c:v>
+                </c:pt>
+                <c:pt idx="4513">
+                  <c:v>41645.0</c:v>
+                </c:pt>
+                <c:pt idx="4514">
+                  <c:v>41645.0</c:v>
+                </c:pt>
+                <c:pt idx="4515">
+                  <c:v>41645.0</c:v>
+                </c:pt>
+                <c:pt idx="4516">
+                  <c:v>41645.0</c:v>
+                </c:pt>
+                <c:pt idx="4517">
+                  <c:v>41645.0</c:v>
+                </c:pt>
+                <c:pt idx="4518">
+                  <c:v>41645.0</c:v>
+                </c:pt>
+                <c:pt idx="4519">
+                  <c:v>41645.0</c:v>
+                </c:pt>
+                <c:pt idx="4520">
+                  <c:v>41645.0</c:v>
+                </c:pt>
+                <c:pt idx="4521">
+                  <c:v>41645.0</c:v>
+                </c:pt>
+                <c:pt idx="4522">
+                  <c:v>41645.0</c:v>
+                </c:pt>
+                <c:pt idx="4523">
+                  <c:v>41645.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SubmissionDates!$B$1:$B$4324</c:f>
+              <c:f>SubmissionDates!$B$1:$B$4524</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4324"/>
+                <c:ptCount val="4524"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -26095,6 +26694,606 @@
                 </c:pt>
                 <c:pt idx="4323">
                   <c:v>4324.0</c:v>
+                </c:pt>
+                <c:pt idx="4324">
+                  <c:v>4325.0</c:v>
+                </c:pt>
+                <c:pt idx="4325">
+                  <c:v>4326.0</c:v>
+                </c:pt>
+                <c:pt idx="4326">
+                  <c:v>4327.0</c:v>
+                </c:pt>
+                <c:pt idx="4327">
+                  <c:v>4328.0</c:v>
+                </c:pt>
+                <c:pt idx="4328">
+                  <c:v>4329.0</c:v>
+                </c:pt>
+                <c:pt idx="4329">
+                  <c:v>4330.0</c:v>
+                </c:pt>
+                <c:pt idx="4330">
+                  <c:v>4331.0</c:v>
+                </c:pt>
+                <c:pt idx="4331">
+                  <c:v>4332.0</c:v>
+                </c:pt>
+                <c:pt idx="4332">
+                  <c:v>4333.0</c:v>
+                </c:pt>
+                <c:pt idx="4333">
+                  <c:v>4334.0</c:v>
+                </c:pt>
+                <c:pt idx="4334">
+                  <c:v>4335.0</c:v>
+                </c:pt>
+                <c:pt idx="4335">
+                  <c:v>4336.0</c:v>
+                </c:pt>
+                <c:pt idx="4336">
+                  <c:v>4337.0</c:v>
+                </c:pt>
+                <c:pt idx="4337">
+                  <c:v>4338.0</c:v>
+                </c:pt>
+                <c:pt idx="4338">
+                  <c:v>4339.0</c:v>
+                </c:pt>
+                <c:pt idx="4339">
+                  <c:v>4340.0</c:v>
+                </c:pt>
+                <c:pt idx="4340">
+                  <c:v>4341.0</c:v>
+                </c:pt>
+                <c:pt idx="4341">
+                  <c:v>4342.0</c:v>
+                </c:pt>
+                <c:pt idx="4342">
+                  <c:v>4343.0</c:v>
+                </c:pt>
+                <c:pt idx="4343">
+                  <c:v>4344.0</c:v>
+                </c:pt>
+                <c:pt idx="4344">
+                  <c:v>4345.0</c:v>
+                </c:pt>
+                <c:pt idx="4345">
+                  <c:v>4346.0</c:v>
+                </c:pt>
+                <c:pt idx="4346">
+                  <c:v>4347.0</c:v>
+                </c:pt>
+                <c:pt idx="4347">
+                  <c:v>4348.0</c:v>
+                </c:pt>
+                <c:pt idx="4348">
+                  <c:v>4349.0</c:v>
+                </c:pt>
+                <c:pt idx="4349">
+                  <c:v>4350.0</c:v>
+                </c:pt>
+                <c:pt idx="4350">
+                  <c:v>4351.0</c:v>
+                </c:pt>
+                <c:pt idx="4351">
+                  <c:v>4352.0</c:v>
+                </c:pt>
+                <c:pt idx="4352">
+                  <c:v>4353.0</c:v>
+                </c:pt>
+                <c:pt idx="4353">
+                  <c:v>4354.0</c:v>
+                </c:pt>
+                <c:pt idx="4354">
+                  <c:v>4355.0</c:v>
+                </c:pt>
+                <c:pt idx="4355">
+                  <c:v>4356.0</c:v>
+                </c:pt>
+                <c:pt idx="4356">
+                  <c:v>4357.0</c:v>
+                </c:pt>
+                <c:pt idx="4357">
+                  <c:v>4358.0</c:v>
+                </c:pt>
+                <c:pt idx="4358">
+                  <c:v>4359.0</c:v>
+                </c:pt>
+                <c:pt idx="4359">
+                  <c:v>4360.0</c:v>
+                </c:pt>
+                <c:pt idx="4360">
+                  <c:v>4361.0</c:v>
+                </c:pt>
+                <c:pt idx="4361">
+                  <c:v>4362.0</c:v>
+                </c:pt>
+                <c:pt idx="4362">
+                  <c:v>4363.0</c:v>
+                </c:pt>
+                <c:pt idx="4363">
+                  <c:v>4364.0</c:v>
+                </c:pt>
+                <c:pt idx="4364">
+                  <c:v>4365.0</c:v>
+                </c:pt>
+                <c:pt idx="4365">
+                  <c:v>4366.0</c:v>
+                </c:pt>
+                <c:pt idx="4366">
+                  <c:v>4367.0</c:v>
+                </c:pt>
+                <c:pt idx="4367">
+                  <c:v>4368.0</c:v>
+                </c:pt>
+                <c:pt idx="4368">
+                  <c:v>4369.0</c:v>
+                </c:pt>
+                <c:pt idx="4369">
+                  <c:v>4370.0</c:v>
+                </c:pt>
+                <c:pt idx="4370">
+                  <c:v>4371.0</c:v>
+                </c:pt>
+                <c:pt idx="4371">
+                  <c:v>4372.0</c:v>
+                </c:pt>
+                <c:pt idx="4372">
+                  <c:v>4373.0</c:v>
+                </c:pt>
+                <c:pt idx="4373">
+                  <c:v>4374.0</c:v>
+                </c:pt>
+                <c:pt idx="4374">
+                  <c:v>4375.0</c:v>
+                </c:pt>
+                <c:pt idx="4375">
+                  <c:v>4376.0</c:v>
+                </c:pt>
+                <c:pt idx="4376">
+                  <c:v>4377.0</c:v>
+                </c:pt>
+                <c:pt idx="4377">
+                  <c:v>4378.0</c:v>
+                </c:pt>
+                <c:pt idx="4378">
+                  <c:v>4379.0</c:v>
+                </c:pt>
+                <c:pt idx="4379">
+                  <c:v>4380.0</c:v>
+                </c:pt>
+                <c:pt idx="4380">
+                  <c:v>4381.0</c:v>
+                </c:pt>
+                <c:pt idx="4381">
+                  <c:v>4382.0</c:v>
+                </c:pt>
+                <c:pt idx="4382">
+                  <c:v>4383.0</c:v>
+                </c:pt>
+                <c:pt idx="4383">
+                  <c:v>4384.0</c:v>
+                </c:pt>
+                <c:pt idx="4384">
+                  <c:v>4385.0</c:v>
+                </c:pt>
+                <c:pt idx="4385">
+                  <c:v>4386.0</c:v>
+                </c:pt>
+                <c:pt idx="4386">
+                  <c:v>4387.0</c:v>
+                </c:pt>
+                <c:pt idx="4387">
+                  <c:v>4388.0</c:v>
+                </c:pt>
+                <c:pt idx="4388">
+                  <c:v>4389.0</c:v>
+                </c:pt>
+                <c:pt idx="4389">
+                  <c:v>4390.0</c:v>
+                </c:pt>
+                <c:pt idx="4390">
+                  <c:v>4391.0</c:v>
+                </c:pt>
+                <c:pt idx="4391">
+                  <c:v>4392.0</c:v>
+                </c:pt>
+                <c:pt idx="4392">
+                  <c:v>4393.0</c:v>
+                </c:pt>
+                <c:pt idx="4393">
+                  <c:v>4394.0</c:v>
+                </c:pt>
+                <c:pt idx="4394">
+                  <c:v>4395.0</c:v>
+                </c:pt>
+                <c:pt idx="4395">
+                  <c:v>4396.0</c:v>
+                </c:pt>
+                <c:pt idx="4396">
+                  <c:v>4397.0</c:v>
+                </c:pt>
+                <c:pt idx="4397">
+                  <c:v>4398.0</c:v>
+                </c:pt>
+                <c:pt idx="4398">
+                  <c:v>4399.0</c:v>
+                </c:pt>
+                <c:pt idx="4399">
+                  <c:v>4400.0</c:v>
+                </c:pt>
+                <c:pt idx="4400">
+                  <c:v>4401.0</c:v>
+                </c:pt>
+                <c:pt idx="4401">
+                  <c:v>4402.0</c:v>
+                </c:pt>
+                <c:pt idx="4402">
+                  <c:v>4403.0</c:v>
+                </c:pt>
+                <c:pt idx="4403">
+                  <c:v>4404.0</c:v>
+                </c:pt>
+                <c:pt idx="4404">
+                  <c:v>4405.0</c:v>
+                </c:pt>
+                <c:pt idx="4405">
+                  <c:v>4406.0</c:v>
+                </c:pt>
+                <c:pt idx="4406">
+                  <c:v>4407.0</c:v>
+                </c:pt>
+                <c:pt idx="4407">
+                  <c:v>4408.0</c:v>
+                </c:pt>
+                <c:pt idx="4408">
+                  <c:v>4409.0</c:v>
+                </c:pt>
+                <c:pt idx="4409">
+                  <c:v>4410.0</c:v>
+                </c:pt>
+                <c:pt idx="4410">
+                  <c:v>4411.0</c:v>
+                </c:pt>
+                <c:pt idx="4411">
+                  <c:v>4412.0</c:v>
+                </c:pt>
+                <c:pt idx="4412">
+                  <c:v>4413.0</c:v>
+                </c:pt>
+                <c:pt idx="4413">
+                  <c:v>4414.0</c:v>
+                </c:pt>
+                <c:pt idx="4414">
+                  <c:v>4415.0</c:v>
+                </c:pt>
+                <c:pt idx="4415">
+                  <c:v>4416.0</c:v>
+                </c:pt>
+                <c:pt idx="4416">
+                  <c:v>4417.0</c:v>
+                </c:pt>
+                <c:pt idx="4417">
+                  <c:v>4418.0</c:v>
+                </c:pt>
+                <c:pt idx="4418">
+                  <c:v>4419.0</c:v>
+                </c:pt>
+                <c:pt idx="4419">
+                  <c:v>4420.0</c:v>
+                </c:pt>
+                <c:pt idx="4420">
+                  <c:v>4421.0</c:v>
+                </c:pt>
+                <c:pt idx="4421">
+                  <c:v>4422.0</c:v>
+                </c:pt>
+                <c:pt idx="4422">
+                  <c:v>4423.0</c:v>
+                </c:pt>
+                <c:pt idx="4423">
+                  <c:v>4424.0</c:v>
+                </c:pt>
+                <c:pt idx="4424">
+                  <c:v>4425.0</c:v>
+                </c:pt>
+                <c:pt idx="4425">
+                  <c:v>4426.0</c:v>
+                </c:pt>
+                <c:pt idx="4426">
+                  <c:v>4427.0</c:v>
+                </c:pt>
+                <c:pt idx="4427">
+                  <c:v>4428.0</c:v>
+                </c:pt>
+                <c:pt idx="4428">
+                  <c:v>4429.0</c:v>
+                </c:pt>
+                <c:pt idx="4429">
+                  <c:v>4430.0</c:v>
+                </c:pt>
+                <c:pt idx="4430">
+                  <c:v>4431.0</c:v>
+                </c:pt>
+                <c:pt idx="4431">
+                  <c:v>4432.0</c:v>
+                </c:pt>
+                <c:pt idx="4432">
+                  <c:v>4433.0</c:v>
+                </c:pt>
+                <c:pt idx="4433">
+                  <c:v>4434.0</c:v>
+                </c:pt>
+                <c:pt idx="4434">
+                  <c:v>4435.0</c:v>
+                </c:pt>
+                <c:pt idx="4435">
+                  <c:v>4436.0</c:v>
+                </c:pt>
+                <c:pt idx="4436">
+                  <c:v>4437.0</c:v>
+                </c:pt>
+                <c:pt idx="4437">
+                  <c:v>4438.0</c:v>
+                </c:pt>
+                <c:pt idx="4438">
+                  <c:v>4439.0</c:v>
+                </c:pt>
+                <c:pt idx="4439">
+                  <c:v>4440.0</c:v>
+                </c:pt>
+                <c:pt idx="4440">
+                  <c:v>4441.0</c:v>
+                </c:pt>
+                <c:pt idx="4441">
+                  <c:v>4442.0</c:v>
+                </c:pt>
+                <c:pt idx="4442">
+                  <c:v>4443.0</c:v>
+                </c:pt>
+                <c:pt idx="4443">
+                  <c:v>4444.0</c:v>
+                </c:pt>
+                <c:pt idx="4444">
+                  <c:v>4445.0</c:v>
+                </c:pt>
+                <c:pt idx="4445">
+                  <c:v>4446.0</c:v>
+                </c:pt>
+                <c:pt idx="4446">
+                  <c:v>4447.0</c:v>
+                </c:pt>
+                <c:pt idx="4447">
+                  <c:v>4448.0</c:v>
+                </c:pt>
+                <c:pt idx="4448">
+                  <c:v>4449.0</c:v>
+                </c:pt>
+                <c:pt idx="4449">
+                  <c:v>4450.0</c:v>
+                </c:pt>
+                <c:pt idx="4450">
+                  <c:v>4451.0</c:v>
+                </c:pt>
+                <c:pt idx="4451">
+                  <c:v>4452.0</c:v>
+                </c:pt>
+                <c:pt idx="4452">
+                  <c:v>4453.0</c:v>
+                </c:pt>
+                <c:pt idx="4453">
+                  <c:v>4454.0</c:v>
+                </c:pt>
+                <c:pt idx="4454">
+                  <c:v>4455.0</c:v>
+                </c:pt>
+                <c:pt idx="4455">
+                  <c:v>4456.0</c:v>
+                </c:pt>
+                <c:pt idx="4456">
+                  <c:v>4457.0</c:v>
+                </c:pt>
+                <c:pt idx="4457">
+                  <c:v>4458.0</c:v>
+                </c:pt>
+                <c:pt idx="4458">
+                  <c:v>4459.0</c:v>
+                </c:pt>
+                <c:pt idx="4459">
+                  <c:v>4460.0</c:v>
+                </c:pt>
+                <c:pt idx="4460">
+                  <c:v>4461.0</c:v>
+                </c:pt>
+                <c:pt idx="4461">
+                  <c:v>4462.0</c:v>
+                </c:pt>
+                <c:pt idx="4462">
+                  <c:v>4463.0</c:v>
+                </c:pt>
+                <c:pt idx="4463">
+                  <c:v>4464.0</c:v>
+                </c:pt>
+                <c:pt idx="4464">
+                  <c:v>4465.0</c:v>
+                </c:pt>
+                <c:pt idx="4465">
+                  <c:v>4466.0</c:v>
+                </c:pt>
+                <c:pt idx="4466">
+                  <c:v>4467.0</c:v>
+                </c:pt>
+                <c:pt idx="4467">
+                  <c:v>4468.0</c:v>
+                </c:pt>
+                <c:pt idx="4468">
+                  <c:v>4469.0</c:v>
+                </c:pt>
+                <c:pt idx="4469">
+                  <c:v>4470.0</c:v>
+                </c:pt>
+                <c:pt idx="4470">
+                  <c:v>4471.0</c:v>
+                </c:pt>
+                <c:pt idx="4471">
+                  <c:v>4472.0</c:v>
+                </c:pt>
+                <c:pt idx="4472">
+                  <c:v>4473.0</c:v>
+                </c:pt>
+                <c:pt idx="4473">
+                  <c:v>4474.0</c:v>
+                </c:pt>
+                <c:pt idx="4474">
+                  <c:v>4475.0</c:v>
+                </c:pt>
+                <c:pt idx="4475">
+                  <c:v>4476.0</c:v>
+                </c:pt>
+                <c:pt idx="4476">
+                  <c:v>4477.0</c:v>
+                </c:pt>
+                <c:pt idx="4477">
+                  <c:v>4478.0</c:v>
+                </c:pt>
+                <c:pt idx="4478">
+                  <c:v>4479.0</c:v>
+                </c:pt>
+                <c:pt idx="4479">
+                  <c:v>4480.0</c:v>
+                </c:pt>
+                <c:pt idx="4480">
+                  <c:v>4481.0</c:v>
+                </c:pt>
+                <c:pt idx="4481">
+                  <c:v>4482.0</c:v>
+                </c:pt>
+                <c:pt idx="4482">
+                  <c:v>4483.0</c:v>
+                </c:pt>
+                <c:pt idx="4483">
+                  <c:v>4484.0</c:v>
+                </c:pt>
+                <c:pt idx="4484">
+                  <c:v>4485.0</c:v>
+                </c:pt>
+                <c:pt idx="4485">
+                  <c:v>4486.0</c:v>
+                </c:pt>
+                <c:pt idx="4486">
+                  <c:v>4487.0</c:v>
+                </c:pt>
+                <c:pt idx="4487">
+                  <c:v>4488.0</c:v>
+                </c:pt>
+                <c:pt idx="4488">
+                  <c:v>4489.0</c:v>
+                </c:pt>
+                <c:pt idx="4489">
+                  <c:v>4490.0</c:v>
+                </c:pt>
+                <c:pt idx="4490">
+                  <c:v>4491.0</c:v>
+                </c:pt>
+                <c:pt idx="4491">
+                  <c:v>4492.0</c:v>
+                </c:pt>
+                <c:pt idx="4492">
+                  <c:v>4493.0</c:v>
+                </c:pt>
+                <c:pt idx="4493">
+                  <c:v>4494.0</c:v>
+                </c:pt>
+                <c:pt idx="4494">
+                  <c:v>4495.0</c:v>
+                </c:pt>
+                <c:pt idx="4495">
+                  <c:v>4496.0</c:v>
+                </c:pt>
+                <c:pt idx="4496">
+                  <c:v>4497.0</c:v>
+                </c:pt>
+                <c:pt idx="4497">
+                  <c:v>4498.0</c:v>
+                </c:pt>
+                <c:pt idx="4498">
+                  <c:v>4499.0</c:v>
+                </c:pt>
+                <c:pt idx="4499">
+                  <c:v>4500.0</c:v>
+                </c:pt>
+                <c:pt idx="4500">
+                  <c:v>4501.0</c:v>
+                </c:pt>
+                <c:pt idx="4501">
+                  <c:v>4502.0</c:v>
+                </c:pt>
+                <c:pt idx="4502">
+                  <c:v>4503.0</c:v>
+                </c:pt>
+                <c:pt idx="4503">
+                  <c:v>4504.0</c:v>
+                </c:pt>
+                <c:pt idx="4504">
+                  <c:v>4505.0</c:v>
+                </c:pt>
+                <c:pt idx="4505">
+                  <c:v>4506.0</c:v>
+                </c:pt>
+                <c:pt idx="4506">
+                  <c:v>4507.0</c:v>
+                </c:pt>
+                <c:pt idx="4507">
+                  <c:v>4508.0</c:v>
+                </c:pt>
+                <c:pt idx="4508">
+                  <c:v>4509.0</c:v>
+                </c:pt>
+                <c:pt idx="4509">
+                  <c:v>4510.0</c:v>
+                </c:pt>
+                <c:pt idx="4510">
+                  <c:v>4511.0</c:v>
+                </c:pt>
+                <c:pt idx="4511">
+                  <c:v>4512.0</c:v>
+                </c:pt>
+                <c:pt idx="4512">
+                  <c:v>4513.0</c:v>
+                </c:pt>
+                <c:pt idx="4513">
+                  <c:v>4514.0</c:v>
+                </c:pt>
+                <c:pt idx="4514">
+                  <c:v>4515.0</c:v>
+                </c:pt>
+                <c:pt idx="4515">
+                  <c:v>4516.0</c:v>
+                </c:pt>
+                <c:pt idx="4516">
+                  <c:v>4517.0</c:v>
+                </c:pt>
+                <c:pt idx="4517">
+                  <c:v>4518.0</c:v>
+                </c:pt>
+                <c:pt idx="4518">
+                  <c:v>4519.0</c:v>
+                </c:pt>
+                <c:pt idx="4519">
+                  <c:v>4520.0</c:v>
+                </c:pt>
+                <c:pt idx="4520">
+                  <c:v>4521.0</c:v>
+                </c:pt>
+                <c:pt idx="4521">
+                  <c:v>4522.0</c:v>
+                </c:pt>
+                <c:pt idx="4522">
+                  <c:v>4523.0</c:v>
+                </c:pt>
+                <c:pt idx="4523">
+                  <c:v>4524.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -26111,11 +27310,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2118566456"/>
-        <c:axId val="2118569496"/>
+        <c:axId val="2032232296"/>
+        <c:axId val="2032226696"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2118566456"/>
+        <c:axId val="2032232296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="41640.0"/>
@@ -26127,7 +27326,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118569496"/>
+        <c:crossAx val="2032226696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
@@ -26138,7 +27337,7 @@
         <c:minorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2118569496"/>
+        <c:axId val="2032226696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26149,7 +27348,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118566456"/>
+        <c:crossAx val="2032232296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -26639,6 +27838,9 @@
                 <c:pt idx="71">
                   <c:v>154.0</c:v>
                 </c:pt>
+                <c:pt idx="72">
+                  <c:v>132.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -26652,11 +27854,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2118893736"/>
-        <c:axId val="2118896744"/>
+        <c:axId val="2106462648"/>
+        <c:axId val="2106465688"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="2118893736"/>
+        <c:axId val="2106462648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26666,14 +27868,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118896744"/>
+        <c:crossAx val="2106465688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2118896744"/>
+        <c:axId val="2106465688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -26684,7 +27886,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2118893736"/>
+        <c:crossAx val="2106462648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -26700,7 +27902,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="146" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="141" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -26712,7 +27914,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="146" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -26724,7 +27926,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8568151" cy="5828082"/>
+    <xdr:ext cx="8565745" cy="5818582"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1" title="Data Packages in Dryad"/>
@@ -26751,7 +27953,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8568028" cy="5822324"/>
+    <xdr:ext cx="8565745" cy="5818582"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -27100,10 +28302,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4374"/>
+  <dimension ref="A1:B4524"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4331" workbookViewId="0">
-      <selection activeCell="D4374" sqref="D4374"/>
+    <sheetView topLeftCell="A4465" workbookViewId="0">
+      <selection activeCell="A4493" sqref="A4493"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -62101,6 +63303,1206 @@
       </c>
       <c r="B4374">
         <v>4374</v>
+      </c>
+    </row>
+    <row r="4375" spans="1:2">
+      <c r="A4375" s="1">
+        <v>41612</v>
+      </c>
+      <c r="B4375">
+        <v>4375</v>
+      </c>
+    </row>
+    <row r="4376" spans="1:2">
+      <c r="A4376" s="1">
+        <v>41612</v>
+      </c>
+      <c r="B4376">
+        <v>4376</v>
+      </c>
+    </row>
+    <row r="4377" spans="1:2">
+      <c r="A4377" s="1">
+        <v>41612</v>
+      </c>
+      <c r="B4377">
+        <v>4377</v>
+      </c>
+    </row>
+    <row r="4378" spans="1:2">
+      <c r="A4378" s="1">
+        <v>41612</v>
+      </c>
+      <c r="B4378">
+        <v>4378</v>
+      </c>
+    </row>
+    <row r="4379" spans="1:2">
+      <c r="A4379" s="1">
+        <v>41613</v>
+      </c>
+      <c r="B4379">
+        <v>4379</v>
+      </c>
+    </row>
+    <row r="4380" spans="1:2">
+      <c r="A4380" s="1">
+        <v>41613</v>
+      </c>
+      <c r="B4380">
+        <v>4380</v>
+      </c>
+    </row>
+    <row r="4381" spans="1:2">
+      <c r="A4381" s="1">
+        <v>41613</v>
+      </c>
+      <c r="B4381">
+        <v>4381</v>
+      </c>
+    </row>
+    <row r="4382" spans="1:2">
+      <c r="A4382" s="1">
+        <v>41613</v>
+      </c>
+      <c r="B4382">
+        <v>4382</v>
+      </c>
+    </row>
+    <row r="4383" spans="1:2">
+      <c r="A4383" s="1">
+        <v>41613</v>
+      </c>
+      <c r="B4383">
+        <v>4383</v>
+      </c>
+    </row>
+    <row r="4384" spans="1:2">
+      <c r="A4384" s="1">
+        <v>41613</v>
+      </c>
+      <c r="B4384">
+        <v>4384</v>
+      </c>
+    </row>
+    <row r="4385" spans="1:2">
+      <c r="A4385" s="1">
+        <v>41613</v>
+      </c>
+      <c r="B4385">
+        <v>4385</v>
+      </c>
+    </row>
+    <row r="4386" spans="1:2">
+      <c r="A4386" s="1">
+        <v>41613</v>
+      </c>
+      <c r="B4386">
+        <v>4386</v>
+      </c>
+    </row>
+    <row r="4387" spans="1:2">
+      <c r="A4387" s="1">
+        <v>41613</v>
+      </c>
+      <c r="B4387">
+        <v>4387</v>
+      </c>
+    </row>
+    <row r="4388" spans="1:2">
+      <c r="A4388" s="1">
+        <v>41613</v>
+      </c>
+      <c r="B4388">
+        <v>4388</v>
+      </c>
+    </row>
+    <row r="4389" spans="1:2">
+      <c r="A4389" s="1">
+        <v>41613</v>
+      </c>
+      <c r="B4389">
+        <v>4389</v>
+      </c>
+    </row>
+    <row r="4390" spans="1:2">
+      <c r="A4390" s="1">
+        <v>41613</v>
+      </c>
+      <c r="B4390">
+        <v>4390</v>
+      </c>
+    </row>
+    <row r="4391" spans="1:2">
+      <c r="A4391" s="1">
+        <v>41613</v>
+      </c>
+      <c r="B4391">
+        <v>4391</v>
+      </c>
+    </row>
+    <row r="4392" spans="1:2">
+      <c r="A4392" s="1">
+        <v>41613</v>
+      </c>
+      <c r="B4392">
+        <v>4392</v>
+      </c>
+    </row>
+    <row r="4393" spans="1:2">
+      <c r="A4393" s="1">
+        <v>41613</v>
+      </c>
+      <c r="B4393">
+        <v>4393</v>
+      </c>
+    </row>
+    <row r="4394" spans="1:2">
+      <c r="A4394" s="1">
+        <v>41614</v>
+      </c>
+      <c r="B4394">
+        <v>4394</v>
+      </c>
+    </row>
+    <row r="4395" spans="1:2">
+      <c r="A4395" s="1">
+        <v>41614</v>
+      </c>
+      <c r="B4395">
+        <v>4395</v>
+      </c>
+    </row>
+    <row r="4396" spans="1:2">
+      <c r="A4396" s="1">
+        <v>41617</v>
+      </c>
+      <c r="B4396">
+        <v>4396</v>
+      </c>
+    </row>
+    <row r="4397" spans="1:2">
+      <c r="A4397" s="1">
+        <v>41617</v>
+      </c>
+      <c r="B4397">
+        <v>4397</v>
+      </c>
+    </row>
+    <row r="4398" spans="1:2">
+      <c r="A4398" s="1">
+        <v>41617</v>
+      </c>
+      <c r="B4398">
+        <v>4398</v>
+      </c>
+    </row>
+    <row r="4399" spans="1:2">
+      <c r="A4399" s="1">
+        <v>41617</v>
+      </c>
+      <c r="B4399">
+        <v>4399</v>
+      </c>
+    </row>
+    <row r="4400" spans="1:2">
+      <c r="A4400" s="1">
+        <v>41617</v>
+      </c>
+      <c r="B4400">
+        <v>4400</v>
+      </c>
+    </row>
+    <row r="4401" spans="1:2">
+      <c r="A4401" s="1">
+        <v>41617</v>
+      </c>
+      <c r="B4401">
+        <v>4401</v>
+      </c>
+    </row>
+    <row r="4402" spans="1:2">
+      <c r="A4402" s="1">
+        <v>41617</v>
+      </c>
+      <c r="B4402">
+        <v>4402</v>
+      </c>
+    </row>
+    <row r="4403" spans="1:2">
+      <c r="A4403" s="1">
+        <v>41617</v>
+      </c>
+      <c r="B4403">
+        <v>4403</v>
+      </c>
+    </row>
+    <row r="4404" spans="1:2">
+      <c r="A4404" s="1">
+        <v>41617</v>
+      </c>
+      <c r="B4404">
+        <v>4404</v>
+      </c>
+    </row>
+    <row r="4405" spans="1:2">
+      <c r="A4405" s="1">
+        <v>41617</v>
+      </c>
+      <c r="B4405">
+        <v>4405</v>
+      </c>
+    </row>
+    <row r="4406" spans="1:2">
+      <c r="A4406" s="1">
+        <v>41617</v>
+      </c>
+      <c r="B4406">
+        <v>4406</v>
+      </c>
+    </row>
+    <row r="4407" spans="1:2">
+      <c r="A4407" s="1">
+        <v>41617</v>
+      </c>
+      <c r="B4407">
+        <v>4407</v>
+      </c>
+    </row>
+    <row r="4408" spans="1:2">
+      <c r="A4408" s="1">
+        <v>41617</v>
+      </c>
+      <c r="B4408">
+        <v>4408</v>
+      </c>
+    </row>
+    <row r="4409" spans="1:2">
+      <c r="A4409" s="1">
+        <v>41617</v>
+      </c>
+      <c r="B4409">
+        <v>4409</v>
+      </c>
+    </row>
+    <row r="4410" spans="1:2">
+      <c r="A4410" s="1">
+        <v>41617</v>
+      </c>
+      <c r="B4410">
+        <v>4410</v>
+      </c>
+    </row>
+    <row r="4411" spans="1:2">
+      <c r="A4411" s="1">
+        <v>41617</v>
+      </c>
+      <c r="B4411">
+        <v>4411</v>
+      </c>
+    </row>
+    <row r="4412" spans="1:2">
+      <c r="A4412" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4412">
+        <v>4412</v>
+      </c>
+    </row>
+    <row r="4413" spans="1:2">
+      <c r="A4413" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4413">
+        <v>4413</v>
+      </c>
+    </row>
+    <row r="4414" spans="1:2">
+      <c r="A4414" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4414">
+        <v>4414</v>
+      </c>
+    </row>
+    <row r="4415" spans="1:2">
+      <c r="A4415" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4415">
+        <v>4415</v>
+      </c>
+    </row>
+    <row r="4416" spans="1:2">
+      <c r="A4416" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4416">
+        <v>4416</v>
+      </c>
+    </row>
+    <row r="4417" spans="1:2">
+      <c r="A4417" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4417">
+        <v>4417</v>
+      </c>
+    </row>
+    <row r="4418" spans="1:2">
+      <c r="A4418" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4418">
+        <v>4418</v>
+      </c>
+    </row>
+    <row r="4419" spans="1:2">
+      <c r="A4419" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4419">
+        <v>4419</v>
+      </c>
+    </row>
+    <row r="4420" spans="1:2">
+      <c r="A4420" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4420">
+        <v>4420</v>
+      </c>
+    </row>
+    <row r="4421" spans="1:2">
+      <c r="A4421" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4421">
+        <v>4421</v>
+      </c>
+    </row>
+    <row r="4422" spans="1:2">
+      <c r="A4422" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4422">
+        <v>4422</v>
+      </c>
+    </row>
+    <row r="4423" spans="1:2">
+      <c r="A4423" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4423">
+        <v>4423</v>
+      </c>
+    </row>
+    <row r="4424" spans="1:2">
+      <c r="A4424" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4424">
+        <v>4424</v>
+      </c>
+    </row>
+    <row r="4425" spans="1:2">
+      <c r="A4425" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4425">
+        <v>4425</v>
+      </c>
+    </row>
+    <row r="4426" spans="1:2">
+      <c r="A4426" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4426">
+        <v>4426</v>
+      </c>
+    </row>
+    <row r="4427" spans="1:2">
+      <c r="A4427" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4427">
+        <v>4427</v>
+      </c>
+    </row>
+    <row r="4428" spans="1:2">
+      <c r="A4428" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4428">
+        <v>4428</v>
+      </c>
+    </row>
+    <row r="4429" spans="1:2">
+      <c r="A4429" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4429">
+        <v>4429</v>
+      </c>
+    </row>
+    <row r="4430" spans="1:2">
+      <c r="A4430" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4430">
+        <v>4430</v>
+      </c>
+    </row>
+    <row r="4431" spans="1:2">
+      <c r="A4431" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4431">
+        <v>4431</v>
+      </c>
+    </row>
+    <row r="4432" spans="1:2">
+      <c r="A4432" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4432">
+        <v>4432</v>
+      </c>
+    </row>
+    <row r="4433" spans="1:2">
+      <c r="A4433" s="1">
+        <v>41618</v>
+      </c>
+      <c r="B4433">
+        <v>4433</v>
+      </c>
+    </row>
+    <row r="4434" spans="1:2">
+      <c r="A4434" s="1">
+        <v>41619</v>
+      </c>
+      <c r="B4434">
+        <v>4434</v>
+      </c>
+    </row>
+    <row r="4435" spans="1:2">
+      <c r="A4435" s="1">
+        <v>41619</v>
+      </c>
+      <c r="B4435">
+        <v>4435</v>
+      </c>
+    </row>
+    <row r="4436" spans="1:2">
+      <c r="A4436" s="1">
+        <v>41619</v>
+      </c>
+      <c r="B4436">
+        <v>4436</v>
+      </c>
+    </row>
+    <row r="4437" spans="1:2">
+      <c r="A4437" s="1">
+        <v>41619</v>
+      </c>
+      <c r="B4437">
+        <v>4437</v>
+      </c>
+    </row>
+    <row r="4438" spans="1:2">
+      <c r="A4438" s="1">
+        <v>41619</v>
+      </c>
+      <c r="B4438">
+        <v>4438</v>
+      </c>
+    </row>
+    <row r="4439" spans="1:2">
+      <c r="A4439" s="1">
+        <v>41619</v>
+      </c>
+      <c r="B4439">
+        <v>4439</v>
+      </c>
+    </row>
+    <row r="4440" spans="1:2">
+      <c r="A4440" s="1">
+        <v>41619</v>
+      </c>
+      <c r="B4440">
+        <v>4440</v>
+      </c>
+    </row>
+    <row r="4441" spans="1:2">
+      <c r="A4441" s="1">
+        <v>41619</v>
+      </c>
+      <c r="B4441">
+        <v>4441</v>
+      </c>
+    </row>
+    <row r="4442" spans="1:2">
+      <c r="A4442" s="1">
+        <v>41620</v>
+      </c>
+      <c r="B4442">
+        <v>4442</v>
+      </c>
+    </row>
+    <row r="4443" spans="1:2">
+      <c r="A4443" s="1">
+        <v>41620</v>
+      </c>
+      <c r="B4443">
+        <v>4443</v>
+      </c>
+    </row>
+    <row r="4444" spans="1:2">
+      <c r="A4444" s="1">
+        <v>41620</v>
+      </c>
+      <c r="B4444">
+        <v>4444</v>
+      </c>
+    </row>
+    <row r="4445" spans="1:2">
+      <c r="A4445" s="1">
+        <v>41620</v>
+      </c>
+      <c r="B4445">
+        <v>4445</v>
+      </c>
+    </row>
+    <row r="4446" spans="1:2">
+      <c r="A4446" s="1">
+        <v>41620</v>
+      </c>
+      <c r="B4446">
+        <v>4446</v>
+      </c>
+    </row>
+    <row r="4447" spans="1:2">
+      <c r="A4447" s="1">
+        <v>41621</v>
+      </c>
+      <c r="B4447">
+        <v>4447</v>
+      </c>
+    </row>
+    <row r="4448" spans="1:2">
+      <c r="A4448" s="1">
+        <v>41621</v>
+      </c>
+      <c r="B4448">
+        <v>4448</v>
+      </c>
+    </row>
+    <row r="4449" spans="1:2">
+      <c r="A4449" s="1">
+        <v>41621</v>
+      </c>
+      <c r="B4449">
+        <v>4449</v>
+      </c>
+    </row>
+    <row r="4450" spans="1:2">
+      <c r="A4450" s="1">
+        <v>41621</v>
+      </c>
+      <c r="B4450">
+        <v>4450</v>
+      </c>
+    </row>
+    <row r="4451" spans="1:2">
+      <c r="A4451" s="1">
+        <v>41621</v>
+      </c>
+      <c r="B4451">
+        <v>4451</v>
+      </c>
+    </row>
+    <row r="4452" spans="1:2">
+      <c r="A4452" s="1">
+        <v>41621</v>
+      </c>
+      <c r="B4452">
+        <v>4452</v>
+      </c>
+    </row>
+    <row r="4453" spans="1:2">
+      <c r="A4453" s="1">
+        <v>41621</v>
+      </c>
+      <c r="B4453">
+        <v>4453</v>
+      </c>
+    </row>
+    <row r="4454" spans="1:2">
+      <c r="A4454" s="1">
+        <v>41621</v>
+      </c>
+      <c r="B4454">
+        <v>4454</v>
+      </c>
+    </row>
+    <row r="4455" spans="1:2">
+      <c r="A4455" s="1">
+        <v>41625</v>
+      </c>
+      <c r="B4455">
+        <v>4455</v>
+      </c>
+    </row>
+    <row r="4456" spans="1:2">
+      <c r="A4456" s="1">
+        <v>41625</v>
+      </c>
+      <c r="B4456">
+        <v>4456</v>
+      </c>
+    </row>
+    <row r="4457" spans="1:2">
+      <c r="A4457" s="1">
+        <v>41625</v>
+      </c>
+      <c r="B4457">
+        <v>4457</v>
+      </c>
+    </row>
+    <row r="4458" spans="1:2">
+      <c r="A4458" s="1">
+        <v>41625</v>
+      </c>
+      <c r="B4458">
+        <v>4458</v>
+      </c>
+    </row>
+    <row r="4459" spans="1:2">
+      <c r="A4459" s="1">
+        <v>41625</v>
+      </c>
+      <c r="B4459">
+        <v>4459</v>
+      </c>
+    </row>
+    <row r="4460" spans="1:2">
+      <c r="A4460" s="1">
+        <v>41625</v>
+      </c>
+      <c r="B4460">
+        <v>4460</v>
+      </c>
+    </row>
+    <row r="4461" spans="1:2">
+      <c r="A4461" s="1">
+        <v>41625</v>
+      </c>
+      <c r="B4461">
+        <v>4461</v>
+      </c>
+    </row>
+    <row r="4462" spans="1:2">
+      <c r="A4462" s="1">
+        <v>41625</v>
+      </c>
+      <c r="B4462">
+        <v>4462</v>
+      </c>
+    </row>
+    <row r="4463" spans="1:2">
+      <c r="A4463" s="1">
+        <v>41625</v>
+      </c>
+      <c r="B4463">
+        <v>4463</v>
+      </c>
+    </row>
+    <row r="4464" spans="1:2">
+      <c r="A4464" s="1">
+        <v>41625</v>
+      </c>
+      <c r="B4464">
+        <v>4464</v>
+      </c>
+    </row>
+    <row r="4465" spans="1:2">
+      <c r="A4465" s="1">
+        <v>41625</v>
+      </c>
+      <c r="B4465">
+        <v>4465</v>
+      </c>
+    </row>
+    <row r="4466" spans="1:2">
+      <c r="A4466" s="1">
+        <v>41625</v>
+      </c>
+      <c r="B4466">
+        <v>4466</v>
+      </c>
+    </row>
+    <row r="4467" spans="1:2">
+      <c r="A4467" s="1">
+        <v>41626</v>
+      </c>
+      <c r="B4467">
+        <v>4467</v>
+      </c>
+    </row>
+    <row r="4468" spans="1:2">
+      <c r="A4468" s="1">
+        <v>41626</v>
+      </c>
+      <c r="B4468">
+        <v>4468</v>
+      </c>
+    </row>
+    <row r="4469" spans="1:2">
+      <c r="A4469" s="1">
+        <v>41626</v>
+      </c>
+      <c r="B4469">
+        <v>4469</v>
+      </c>
+    </row>
+    <row r="4470" spans="1:2">
+      <c r="A4470" s="1">
+        <v>41626</v>
+      </c>
+      <c r="B4470">
+        <v>4470</v>
+      </c>
+    </row>
+    <row r="4471" spans="1:2">
+      <c r="A4471" s="1">
+        <v>41626</v>
+      </c>
+      <c r="B4471">
+        <v>4471</v>
+      </c>
+    </row>
+    <row r="4472" spans="1:2">
+      <c r="A4472" s="1">
+        <v>41626</v>
+      </c>
+      <c r="B4472">
+        <v>4472</v>
+      </c>
+    </row>
+    <row r="4473" spans="1:2">
+      <c r="A4473" s="1">
+        <v>41626</v>
+      </c>
+      <c r="B4473">
+        <v>4473</v>
+      </c>
+    </row>
+    <row r="4474" spans="1:2">
+      <c r="A4474" s="1">
+        <v>41627</v>
+      </c>
+      <c r="B4474">
+        <v>4474</v>
+      </c>
+    </row>
+    <row r="4475" spans="1:2">
+      <c r="A4475" s="1">
+        <v>41627</v>
+      </c>
+      <c r="B4475">
+        <v>4475</v>
+      </c>
+    </row>
+    <row r="4476" spans="1:2">
+      <c r="A4476" s="1">
+        <v>41627</v>
+      </c>
+      <c r="B4476">
+        <v>4476</v>
+      </c>
+    </row>
+    <row r="4477" spans="1:2">
+      <c r="A4477" s="1">
+        <v>41627</v>
+      </c>
+      <c r="B4477">
+        <v>4477</v>
+      </c>
+    </row>
+    <row r="4478" spans="1:2">
+      <c r="A4478" s="1">
+        <v>41628</v>
+      </c>
+      <c r="B4478">
+        <v>4478</v>
+      </c>
+    </row>
+    <row r="4479" spans="1:2">
+      <c r="A4479" s="1">
+        <v>41628</v>
+      </c>
+      <c r="B4479">
+        <v>4479</v>
+      </c>
+    </row>
+    <row r="4480" spans="1:2">
+      <c r="A4480" s="1">
+        <v>41628</v>
+      </c>
+      <c r="B4480">
+        <v>4480</v>
+      </c>
+    </row>
+    <row r="4481" spans="1:2">
+      <c r="A4481" s="1">
+        <v>41628</v>
+      </c>
+      <c r="B4481">
+        <v>4481</v>
+      </c>
+    </row>
+    <row r="4482" spans="1:2">
+      <c r="A4482" s="1">
+        <v>41628</v>
+      </c>
+      <c r="B4482">
+        <v>4482</v>
+      </c>
+    </row>
+    <row r="4483" spans="1:2">
+      <c r="A4483" s="1">
+        <v>41628</v>
+      </c>
+      <c r="B4483">
+        <v>4483</v>
+      </c>
+    </row>
+    <row r="4484" spans="1:2">
+      <c r="A4484" s="1">
+        <v>41628</v>
+      </c>
+      <c r="B4484">
+        <v>4484</v>
+      </c>
+    </row>
+    <row r="4485" spans="1:2">
+      <c r="A4485" s="1">
+        <v>41631</v>
+      </c>
+      <c r="B4485">
+        <v>4485</v>
+      </c>
+    </row>
+    <row r="4486" spans="1:2">
+      <c r="A4486" s="1">
+        <v>41631</v>
+      </c>
+      <c r="B4486">
+        <v>4486</v>
+      </c>
+    </row>
+    <row r="4487" spans="1:2">
+      <c r="A4487" s="1">
+        <v>41631</v>
+      </c>
+      <c r="B4487">
+        <v>4487</v>
+      </c>
+    </row>
+    <row r="4488" spans="1:2">
+      <c r="A4488" s="1">
+        <v>41635</v>
+      </c>
+      <c r="B4488">
+        <v>4488</v>
+      </c>
+    </row>
+    <row r="4489" spans="1:2">
+      <c r="A4489" s="1">
+        <v>41635</v>
+      </c>
+      <c r="B4489">
+        <v>4489</v>
+      </c>
+    </row>
+    <row r="4490" spans="1:2">
+      <c r="A4490" s="1">
+        <v>41635</v>
+      </c>
+      <c r="B4490">
+        <v>4490</v>
+      </c>
+    </row>
+    <row r="4491" spans="1:2">
+      <c r="A4491" s="1">
+        <v>41635</v>
+      </c>
+      <c r="B4491">
+        <v>4491</v>
+      </c>
+    </row>
+    <row r="4492" spans="1:2">
+      <c r="A4492" s="1">
+        <v>41635</v>
+      </c>
+      <c r="B4492">
+        <v>4492</v>
+      </c>
+    </row>
+    <row r="4493" spans="1:2">
+      <c r="A4493" s="1">
+        <v>41638</v>
+      </c>
+      <c r="B4493">
+        <v>4493</v>
+      </c>
+    </row>
+    <row r="4494" spans="1:2">
+      <c r="A4494" s="1">
+        <v>41640</v>
+      </c>
+      <c r="B4494">
+        <v>4494</v>
+      </c>
+    </row>
+    <row r="4495" spans="1:2">
+      <c r="A4495" s="1">
+        <v>41641</v>
+      </c>
+      <c r="B4495">
+        <v>4495</v>
+      </c>
+    </row>
+    <row r="4496" spans="1:2">
+      <c r="A4496" s="1">
+        <v>41641</v>
+      </c>
+      <c r="B4496">
+        <v>4496</v>
+      </c>
+    </row>
+    <row r="4497" spans="1:2">
+      <c r="A4497" s="1">
+        <v>41641</v>
+      </c>
+      <c r="B4497">
+        <v>4497</v>
+      </c>
+    </row>
+    <row r="4498" spans="1:2">
+      <c r="A4498" s="1">
+        <v>41641</v>
+      </c>
+      <c r="B4498">
+        <v>4498</v>
+      </c>
+    </row>
+    <row r="4499" spans="1:2">
+      <c r="A4499" s="1">
+        <v>41641</v>
+      </c>
+      <c r="B4499">
+        <v>4499</v>
+      </c>
+    </row>
+    <row r="4500" spans="1:2">
+      <c r="A4500" s="1">
+        <v>41641</v>
+      </c>
+      <c r="B4500">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="4501" spans="1:2">
+      <c r="A4501" s="1">
+        <v>41641</v>
+      </c>
+      <c r="B4501">
+        <v>4501</v>
+      </c>
+    </row>
+    <row r="4502" spans="1:2">
+      <c r="A4502" s="1">
+        <v>41641</v>
+      </c>
+      <c r="B4502">
+        <v>4502</v>
+      </c>
+    </row>
+    <row r="4503" spans="1:2">
+      <c r="A4503" s="1">
+        <v>41641</v>
+      </c>
+      <c r="B4503">
+        <v>4503</v>
+      </c>
+    </row>
+    <row r="4504" spans="1:2">
+      <c r="A4504" s="1">
+        <v>41641</v>
+      </c>
+      <c r="B4504">
+        <v>4504</v>
+      </c>
+    </row>
+    <row r="4505" spans="1:2">
+      <c r="A4505" s="1">
+        <v>41641</v>
+      </c>
+      <c r="B4505">
+        <v>4505</v>
+      </c>
+    </row>
+    <row r="4506" spans="1:2">
+      <c r="A4506" s="1">
+        <v>41641</v>
+      </c>
+      <c r="B4506">
+        <v>4506</v>
+      </c>
+    </row>
+    <row r="4507" spans="1:2">
+      <c r="A4507" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B4507">
+        <v>4507</v>
+      </c>
+    </row>
+    <row r="4508" spans="1:2">
+      <c r="A4508" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B4508">
+        <v>4508</v>
+      </c>
+    </row>
+    <row r="4509" spans="1:2">
+      <c r="A4509" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B4509">
+        <v>4509</v>
+      </c>
+    </row>
+    <row r="4510" spans="1:2">
+      <c r="A4510" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B4510">
+        <v>4510</v>
+      </c>
+    </row>
+    <row r="4511" spans="1:2">
+      <c r="A4511" s="1">
+        <v>41642</v>
+      </c>
+      <c r="B4511">
+        <v>4511</v>
+      </c>
+    </row>
+    <row r="4512" spans="1:2">
+      <c r="A4512" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B4512">
+        <v>4512</v>
+      </c>
+    </row>
+    <row r="4513" spans="1:2">
+      <c r="A4513" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B4513">
+        <v>4513</v>
+      </c>
+    </row>
+    <row r="4514" spans="1:2">
+      <c r="A4514" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B4514">
+        <v>4514</v>
+      </c>
+    </row>
+    <row r="4515" spans="1:2">
+      <c r="A4515" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B4515">
+        <v>4515</v>
+      </c>
+    </row>
+    <row r="4516" spans="1:2">
+      <c r="A4516" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B4516">
+        <v>4516</v>
+      </c>
+    </row>
+    <row r="4517" spans="1:2">
+      <c r="A4517" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B4517">
+        <v>4517</v>
+      </c>
+    </row>
+    <row r="4518" spans="1:2">
+      <c r="A4518" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B4518">
+        <v>4518</v>
+      </c>
+    </row>
+    <row r="4519" spans="1:2">
+      <c r="A4519" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B4519">
+        <v>4519</v>
+      </c>
+    </row>
+    <row r="4520" spans="1:2">
+      <c r="A4520" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B4520">
+        <v>4520</v>
+      </c>
+    </row>
+    <row r="4521" spans="1:2">
+      <c r="A4521" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B4521">
+        <v>4521</v>
+      </c>
+    </row>
+    <row r="4522" spans="1:2">
+      <c r="A4522" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B4522">
+        <v>4522</v>
+      </c>
+    </row>
+    <row r="4523" spans="1:2">
+      <c r="A4523" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B4523">
+        <v>4523</v>
+      </c>
+    </row>
+    <row r="4524" spans="1:2">
+      <c r="A4524" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B4524">
+        <v>4524</v>
       </c>
     </row>
   </sheetData>
@@ -62120,7 +64522,7 @@
   <dimension ref="A1:B74"/>
   <sheetViews>
     <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+      <selection activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -62704,6 +65106,9 @@
     <row r="73" spans="1:2">
       <c r="A73" s="1">
         <v>41609</v>
+      </c>
+      <c r="B73">
+        <v>132</v>
       </c>
     </row>
     <row r="74" spans="1:2">

</xml_diff>

<commit_message>
Update for January 2014
</commit_message>
<xml_diff>
--- a/dataPackages/dataPackagesInDryad.xlsx
+++ b/dataPackages/dataPackagesInDryad.xlsx
@@ -4,16 +4,17 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" checkCompatibility="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="17740" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16480" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="SubmissionDates" sheetId="2" r:id="rId1"/>
-    <sheet name="CumulativeChart" sheetId="3" r:id="rId2"/>
+    <sheet name="CumulativeChart" sheetId="6" r:id="rId2"/>
     <sheet name="SubmissionsPerMonth" sheetId="4" r:id="rId3"/>
     <sheet name="PerMonthChart" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="dryadSubmitDates" localSheetId="0">SubmissionDates!$A$1:$A$4247</definedName>
+    <definedName name="x" localSheetId="0">SubmissionDates!$A$4512:$A$4701</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -28,6 +29,13 @@
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="dryadSubmitDates.txt" type="6" refreshedVersion="0" background="1" saveData="1">
     <textPr fileType="mac" sourceFile="Macintosh HD:Users:ryan:temp:dryadSubmitDates.txt">
+      <textFields>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="2" name="x.txt" type="6" refreshedVersion="0" background="1" saveData="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:ryan:lib:dryad-data:dataPackages:x.txt">
       <textFields>
         <textField/>
       </textFields>
@@ -88,8 +96,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -97,9 +107,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -138,10 +150,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>SubmissionDates!$A$1:$A$4524</c:f>
+              <c:f>SubmissionDates!$A$1:$A$4701</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yy</c:formatCode>
-                <c:ptCount val="4524"/>
+                <c:ptCount val="4701"/>
                 <c:pt idx="0">
                   <c:v>39422.0</c:v>
                 </c:pt>
@@ -13713,16 +13725,547 @@
                 </c:pt>
                 <c:pt idx="4523">
                   <c:v>41645.0</c:v>
+                </c:pt>
+                <c:pt idx="4524">
+                  <c:v>41645.0</c:v>
+                </c:pt>
+                <c:pt idx="4525">
+                  <c:v>41646.0</c:v>
+                </c:pt>
+                <c:pt idx="4526">
+                  <c:v>41646.0</c:v>
+                </c:pt>
+                <c:pt idx="4527">
+                  <c:v>41646.0</c:v>
+                </c:pt>
+                <c:pt idx="4528">
+                  <c:v>41646.0</c:v>
+                </c:pt>
+                <c:pt idx="4529">
+                  <c:v>41646.0</c:v>
+                </c:pt>
+                <c:pt idx="4530">
+                  <c:v>41646.0</c:v>
+                </c:pt>
+                <c:pt idx="4531">
+                  <c:v>41646.0</c:v>
+                </c:pt>
+                <c:pt idx="4532">
+                  <c:v>41646.0</c:v>
+                </c:pt>
+                <c:pt idx="4533">
+                  <c:v>41646.0</c:v>
+                </c:pt>
+                <c:pt idx="4534">
+                  <c:v>41646.0</c:v>
+                </c:pt>
+                <c:pt idx="4535">
+                  <c:v>41646.0</c:v>
+                </c:pt>
+                <c:pt idx="4536">
+                  <c:v>41646.0</c:v>
+                </c:pt>
+                <c:pt idx="4537">
+                  <c:v>41646.0</c:v>
+                </c:pt>
+                <c:pt idx="4538">
+                  <c:v>41646.0</c:v>
+                </c:pt>
+                <c:pt idx="4539">
+                  <c:v>41647.0</c:v>
+                </c:pt>
+                <c:pt idx="4540">
+                  <c:v>41647.0</c:v>
+                </c:pt>
+                <c:pt idx="4541">
+                  <c:v>41647.0</c:v>
+                </c:pt>
+                <c:pt idx="4542">
+                  <c:v>41647.0</c:v>
+                </c:pt>
+                <c:pt idx="4543">
+                  <c:v>41647.0</c:v>
+                </c:pt>
+                <c:pt idx="4544">
+                  <c:v>41647.0</c:v>
+                </c:pt>
+                <c:pt idx="4545">
+                  <c:v>41647.0</c:v>
+                </c:pt>
+                <c:pt idx="4546">
+                  <c:v>41647.0</c:v>
+                </c:pt>
+                <c:pt idx="4547">
+                  <c:v>41647.0</c:v>
+                </c:pt>
+                <c:pt idx="4548">
+                  <c:v>41647.0</c:v>
+                </c:pt>
+                <c:pt idx="4549">
+                  <c:v>41648.0</c:v>
+                </c:pt>
+                <c:pt idx="4550">
+                  <c:v>41648.0</c:v>
+                </c:pt>
+                <c:pt idx="4551">
+                  <c:v>41648.0</c:v>
+                </c:pt>
+                <c:pt idx="4552">
+                  <c:v>41648.0</c:v>
+                </c:pt>
+                <c:pt idx="4553">
+                  <c:v>41648.0</c:v>
+                </c:pt>
+                <c:pt idx="4554">
+                  <c:v>41648.0</c:v>
+                </c:pt>
+                <c:pt idx="4555">
+                  <c:v>41648.0</c:v>
+                </c:pt>
+                <c:pt idx="4556">
+                  <c:v>41649.0</c:v>
+                </c:pt>
+                <c:pt idx="4557">
+                  <c:v>41649.0</c:v>
+                </c:pt>
+                <c:pt idx="4558">
+                  <c:v>41649.0</c:v>
+                </c:pt>
+                <c:pt idx="4559">
+                  <c:v>41649.0</c:v>
+                </c:pt>
+                <c:pt idx="4560">
+                  <c:v>41649.0</c:v>
+                </c:pt>
+                <c:pt idx="4561">
+                  <c:v>41649.0</c:v>
+                </c:pt>
+                <c:pt idx="4562">
+                  <c:v>41649.0</c:v>
+                </c:pt>
+                <c:pt idx="4563">
+                  <c:v>41652.0</c:v>
+                </c:pt>
+                <c:pt idx="4564">
+                  <c:v>41652.0</c:v>
+                </c:pt>
+                <c:pt idx="4565">
+                  <c:v>41652.0</c:v>
+                </c:pt>
+                <c:pt idx="4566">
+                  <c:v>41652.0</c:v>
+                </c:pt>
+                <c:pt idx="4567">
+                  <c:v>41652.0</c:v>
+                </c:pt>
+                <c:pt idx="4568">
+                  <c:v>41653.0</c:v>
+                </c:pt>
+                <c:pt idx="4569">
+                  <c:v>41653.0</c:v>
+                </c:pt>
+                <c:pt idx="4570">
+                  <c:v>41653.0</c:v>
+                </c:pt>
+                <c:pt idx="4571">
+                  <c:v>41653.0</c:v>
+                </c:pt>
+                <c:pt idx="4572">
+                  <c:v>41653.0</c:v>
+                </c:pt>
+                <c:pt idx="4573">
+                  <c:v>41653.0</c:v>
+                </c:pt>
+                <c:pt idx="4574">
+                  <c:v>41653.0</c:v>
+                </c:pt>
+                <c:pt idx="4575">
+                  <c:v>41653.0</c:v>
+                </c:pt>
+                <c:pt idx="4576">
+                  <c:v>41653.0</c:v>
+                </c:pt>
+                <c:pt idx="4577">
+                  <c:v>41653.0</c:v>
+                </c:pt>
+                <c:pt idx="4578">
+                  <c:v>41653.0</c:v>
+                </c:pt>
+                <c:pt idx="4579">
+                  <c:v>41653.0</c:v>
+                </c:pt>
+                <c:pt idx="4580">
+                  <c:v>41653.0</c:v>
+                </c:pt>
+                <c:pt idx="4581">
+                  <c:v>41653.0</c:v>
+                </c:pt>
+                <c:pt idx="4582">
+                  <c:v>41653.0</c:v>
+                </c:pt>
+                <c:pt idx="4583">
+                  <c:v>41653.0</c:v>
+                </c:pt>
+                <c:pt idx="4584">
+                  <c:v>41653.0</c:v>
+                </c:pt>
+                <c:pt idx="4585">
+                  <c:v>41653.0</c:v>
+                </c:pt>
+                <c:pt idx="4586">
+                  <c:v>41654.0</c:v>
+                </c:pt>
+                <c:pt idx="4587">
+                  <c:v>41654.0</c:v>
+                </c:pt>
+                <c:pt idx="4588">
+                  <c:v>41654.0</c:v>
+                </c:pt>
+                <c:pt idx="4589">
+                  <c:v>41654.0</c:v>
+                </c:pt>
+                <c:pt idx="4590">
+                  <c:v>41654.0</c:v>
+                </c:pt>
+                <c:pt idx="4591">
+                  <c:v>41654.0</c:v>
+                </c:pt>
+                <c:pt idx="4592">
+                  <c:v>41654.0</c:v>
+                </c:pt>
+                <c:pt idx="4593">
+                  <c:v>41654.0</c:v>
+                </c:pt>
+                <c:pt idx="4594">
+                  <c:v>41654.0</c:v>
+                </c:pt>
+                <c:pt idx="4595">
+                  <c:v>41654.0</c:v>
+                </c:pt>
+                <c:pt idx="4596">
+                  <c:v>41654.0</c:v>
+                </c:pt>
+                <c:pt idx="4597">
+                  <c:v>41654.0</c:v>
+                </c:pt>
+                <c:pt idx="4598">
+                  <c:v>41654.0</c:v>
+                </c:pt>
+                <c:pt idx="4599">
+                  <c:v>41655.0</c:v>
+                </c:pt>
+                <c:pt idx="4600">
+                  <c:v>41655.0</c:v>
+                </c:pt>
+                <c:pt idx="4601">
+                  <c:v>41655.0</c:v>
+                </c:pt>
+                <c:pt idx="4602">
+                  <c:v>41655.0</c:v>
+                </c:pt>
+                <c:pt idx="4603">
+                  <c:v>41656.0</c:v>
+                </c:pt>
+                <c:pt idx="4604">
+                  <c:v>41656.0</c:v>
+                </c:pt>
+                <c:pt idx="4605">
+                  <c:v>41656.0</c:v>
+                </c:pt>
+                <c:pt idx="4606">
+                  <c:v>41656.0</c:v>
+                </c:pt>
+                <c:pt idx="4607">
+                  <c:v>41660.0</c:v>
+                </c:pt>
+                <c:pt idx="4608">
+                  <c:v>41660.0</c:v>
+                </c:pt>
+                <c:pt idx="4609">
+                  <c:v>41660.0</c:v>
+                </c:pt>
+                <c:pt idx="4610">
+                  <c:v>41660.0</c:v>
+                </c:pt>
+                <c:pt idx="4611">
+                  <c:v>41660.0</c:v>
+                </c:pt>
+                <c:pt idx="4612">
+                  <c:v>41660.0</c:v>
+                </c:pt>
+                <c:pt idx="4613">
+                  <c:v>41660.0</c:v>
+                </c:pt>
+                <c:pt idx="4614">
+                  <c:v>41660.0</c:v>
+                </c:pt>
+                <c:pt idx="4615">
+                  <c:v>41660.0</c:v>
+                </c:pt>
+                <c:pt idx="4616">
+                  <c:v>41660.0</c:v>
+                </c:pt>
+                <c:pt idx="4617">
+                  <c:v>41660.0</c:v>
+                </c:pt>
+                <c:pt idx="4618">
+                  <c:v>41660.0</c:v>
+                </c:pt>
+                <c:pt idx="4619">
+                  <c:v>41660.0</c:v>
+                </c:pt>
+                <c:pt idx="4620">
+                  <c:v>41660.0</c:v>
+                </c:pt>
+                <c:pt idx="4621">
+                  <c:v>41660.0</c:v>
+                </c:pt>
+                <c:pt idx="4622">
+                  <c:v>41660.0</c:v>
+                </c:pt>
+                <c:pt idx="4623">
+                  <c:v>41660.0</c:v>
+                </c:pt>
+                <c:pt idx="4624">
+                  <c:v>41660.0</c:v>
+                </c:pt>
+                <c:pt idx="4625">
+                  <c:v>41660.0</c:v>
+                </c:pt>
+                <c:pt idx="4626">
+                  <c:v>41660.0</c:v>
+                </c:pt>
+                <c:pt idx="4627">
+                  <c:v>41661.0</c:v>
+                </c:pt>
+                <c:pt idx="4628">
+                  <c:v>41661.0</c:v>
+                </c:pt>
+                <c:pt idx="4629">
+                  <c:v>41661.0</c:v>
+                </c:pt>
+                <c:pt idx="4630">
+                  <c:v>41661.0</c:v>
+                </c:pt>
+                <c:pt idx="4631">
+                  <c:v>41661.0</c:v>
+                </c:pt>
+                <c:pt idx="4632">
+                  <c:v>41661.0</c:v>
+                </c:pt>
+                <c:pt idx="4633">
+                  <c:v>41661.0</c:v>
+                </c:pt>
+                <c:pt idx="4634">
+                  <c:v>41661.0</c:v>
+                </c:pt>
+                <c:pt idx="4635">
+                  <c:v>41661.0</c:v>
+                </c:pt>
+                <c:pt idx="4636">
+                  <c:v>41661.0</c:v>
+                </c:pt>
+                <c:pt idx="4637">
+                  <c:v>41661.0</c:v>
+                </c:pt>
+                <c:pt idx="4638">
+                  <c:v>41661.0</c:v>
+                </c:pt>
+                <c:pt idx="4639">
+                  <c:v>41661.0</c:v>
+                </c:pt>
+                <c:pt idx="4640">
+                  <c:v>41662.0</c:v>
+                </c:pt>
+                <c:pt idx="4641">
+                  <c:v>41662.0</c:v>
+                </c:pt>
+                <c:pt idx="4642">
+                  <c:v>41662.0</c:v>
+                </c:pt>
+                <c:pt idx="4643">
+                  <c:v>41662.0</c:v>
+                </c:pt>
+                <c:pt idx="4644">
+                  <c:v>41662.0</c:v>
+                </c:pt>
+                <c:pt idx="4645">
+                  <c:v>41662.0</c:v>
+                </c:pt>
+                <c:pt idx="4646">
+                  <c:v>41663.0</c:v>
+                </c:pt>
+                <c:pt idx="4647">
+                  <c:v>41663.0</c:v>
+                </c:pt>
+                <c:pt idx="4648">
+                  <c:v>41663.0</c:v>
+                </c:pt>
+                <c:pt idx="4649">
+                  <c:v>41663.0</c:v>
+                </c:pt>
+                <c:pt idx="4650">
+                  <c:v>41666.0</c:v>
+                </c:pt>
+                <c:pt idx="4651">
+                  <c:v>41666.0</c:v>
+                </c:pt>
+                <c:pt idx="4652">
+                  <c:v>41666.0</c:v>
+                </c:pt>
+                <c:pt idx="4653">
+                  <c:v>41666.0</c:v>
+                </c:pt>
+                <c:pt idx="4654">
+                  <c:v>41666.0</c:v>
+                </c:pt>
+                <c:pt idx="4655">
+                  <c:v>41666.0</c:v>
+                </c:pt>
+                <c:pt idx="4656">
+                  <c:v>41666.0</c:v>
+                </c:pt>
+                <c:pt idx="4657">
+                  <c:v>41666.0</c:v>
+                </c:pt>
+                <c:pt idx="4658">
+                  <c:v>41666.0</c:v>
+                </c:pt>
+                <c:pt idx="4659">
+                  <c:v>41666.0</c:v>
+                </c:pt>
+                <c:pt idx="4660">
+                  <c:v>41666.0</c:v>
+                </c:pt>
+                <c:pt idx="4661">
+                  <c:v>41666.0</c:v>
+                </c:pt>
+                <c:pt idx="4662">
+                  <c:v>41666.0</c:v>
+                </c:pt>
+                <c:pt idx="4663">
+                  <c:v>41666.0</c:v>
+                </c:pt>
+                <c:pt idx="4664">
+                  <c:v>41666.0</c:v>
+                </c:pt>
+                <c:pt idx="4665">
+                  <c:v>41666.0</c:v>
+                </c:pt>
+                <c:pt idx="4666">
+                  <c:v>41666.0</c:v>
+                </c:pt>
+                <c:pt idx="4667">
+                  <c:v>41666.0</c:v>
+                </c:pt>
+                <c:pt idx="4668">
+                  <c:v>41666.0</c:v>
+                </c:pt>
+                <c:pt idx="4669">
+                  <c:v>41666.0</c:v>
+                </c:pt>
+                <c:pt idx="4670">
+                  <c:v>41667.0</c:v>
+                </c:pt>
+                <c:pt idx="4671">
+                  <c:v>41667.0</c:v>
+                </c:pt>
+                <c:pt idx="4672">
+                  <c:v>41667.0</c:v>
+                </c:pt>
+                <c:pt idx="4673">
+                  <c:v>41667.0</c:v>
+                </c:pt>
+                <c:pt idx="4674">
+                  <c:v>41667.0</c:v>
+                </c:pt>
+                <c:pt idx="4675">
+                  <c:v>41667.0</c:v>
+                </c:pt>
+                <c:pt idx="4676">
+                  <c:v>41667.0</c:v>
+                </c:pt>
+                <c:pt idx="4677">
+                  <c:v>41667.0</c:v>
+                </c:pt>
+                <c:pt idx="4678">
+                  <c:v>41667.0</c:v>
+                </c:pt>
+                <c:pt idx="4679">
+                  <c:v>41667.0</c:v>
+                </c:pt>
+                <c:pt idx="4680">
+                  <c:v>41667.0</c:v>
+                </c:pt>
+                <c:pt idx="4681">
+                  <c:v>41668.0</c:v>
+                </c:pt>
+                <c:pt idx="4682">
+                  <c:v>41668.0</c:v>
+                </c:pt>
+                <c:pt idx="4683">
+                  <c:v>41668.0</c:v>
+                </c:pt>
+                <c:pt idx="4684">
+                  <c:v>41668.0</c:v>
+                </c:pt>
+                <c:pt idx="4685">
+                  <c:v>41668.0</c:v>
+                </c:pt>
+                <c:pt idx="4686">
+                  <c:v>41668.0</c:v>
+                </c:pt>
+                <c:pt idx="4687">
+                  <c:v>41668.0</c:v>
+                </c:pt>
+                <c:pt idx="4688">
+                  <c:v>41668.0</c:v>
+                </c:pt>
+                <c:pt idx="4689">
+                  <c:v>41668.0</c:v>
+                </c:pt>
+                <c:pt idx="4690">
+                  <c:v>41668.0</c:v>
+                </c:pt>
+                <c:pt idx="4691">
+                  <c:v>41668.0</c:v>
+                </c:pt>
+                <c:pt idx="4692">
+                  <c:v>41669.0</c:v>
+                </c:pt>
+                <c:pt idx="4693">
+                  <c:v>41669.0</c:v>
+                </c:pt>
+                <c:pt idx="4694">
+                  <c:v>41669.0</c:v>
+                </c:pt>
+                <c:pt idx="4695">
+                  <c:v>41669.0</c:v>
+                </c:pt>
+                <c:pt idx="4696">
+                  <c:v>41669.0</c:v>
+                </c:pt>
+                <c:pt idx="4697">
+                  <c:v>41670.0</c:v>
+                </c:pt>
+                <c:pt idx="4698">
+                  <c:v>41670.0</c:v>
+                </c:pt>
+                <c:pt idx="4699">
+                  <c:v>41670.0</c:v>
+                </c:pt>
+                <c:pt idx="4700">
+                  <c:v>41670.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>SubmissionDates!$B$1:$B$4524</c:f>
+              <c:f>SubmissionDates!$B$1:$B$4701</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4524"/>
+                <c:ptCount val="4701"/>
                 <c:pt idx="0">
                   <c:v>1.0</c:v>
                 </c:pt>
@@ -27294,6 +27837,537 @@
                 </c:pt>
                 <c:pt idx="4523">
                   <c:v>4524.0</c:v>
+                </c:pt>
+                <c:pt idx="4524">
+                  <c:v>4525.0</c:v>
+                </c:pt>
+                <c:pt idx="4525">
+                  <c:v>4526.0</c:v>
+                </c:pt>
+                <c:pt idx="4526">
+                  <c:v>4527.0</c:v>
+                </c:pt>
+                <c:pt idx="4527">
+                  <c:v>4528.0</c:v>
+                </c:pt>
+                <c:pt idx="4528">
+                  <c:v>4529.0</c:v>
+                </c:pt>
+                <c:pt idx="4529">
+                  <c:v>4530.0</c:v>
+                </c:pt>
+                <c:pt idx="4530">
+                  <c:v>4531.0</c:v>
+                </c:pt>
+                <c:pt idx="4531">
+                  <c:v>4532.0</c:v>
+                </c:pt>
+                <c:pt idx="4532">
+                  <c:v>4533.0</c:v>
+                </c:pt>
+                <c:pt idx="4533">
+                  <c:v>4534.0</c:v>
+                </c:pt>
+                <c:pt idx="4534">
+                  <c:v>4535.0</c:v>
+                </c:pt>
+                <c:pt idx="4535">
+                  <c:v>4536.0</c:v>
+                </c:pt>
+                <c:pt idx="4536">
+                  <c:v>4537.0</c:v>
+                </c:pt>
+                <c:pt idx="4537">
+                  <c:v>4538.0</c:v>
+                </c:pt>
+                <c:pt idx="4538">
+                  <c:v>4539.0</c:v>
+                </c:pt>
+                <c:pt idx="4539">
+                  <c:v>4540.0</c:v>
+                </c:pt>
+                <c:pt idx="4540">
+                  <c:v>4541.0</c:v>
+                </c:pt>
+                <c:pt idx="4541">
+                  <c:v>4542.0</c:v>
+                </c:pt>
+                <c:pt idx="4542">
+                  <c:v>4543.0</c:v>
+                </c:pt>
+                <c:pt idx="4543">
+                  <c:v>4544.0</c:v>
+                </c:pt>
+                <c:pt idx="4544">
+                  <c:v>4545.0</c:v>
+                </c:pt>
+                <c:pt idx="4545">
+                  <c:v>4546.0</c:v>
+                </c:pt>
+                <c:pt idx="4546">
+                  <c:v>4547.0</c:v>
+                </c:pt>
+                <c:pt idx="4547">
+                  <c:v>4548.0</c:v>
+                </c:pt>
+                <c:pt idx="4548">
+                  <c:v>4549.0</c:v>
+                </c:pt>
+                <c:pt idx="4549">
+                  <c:v>4550.0</c:v>
+                </c:pt>
+                <c:pt idx="4550">
+                  <c:v>4551.0</c:v>
+                </c:pt>
+                <c:pt idx="4551">
+                  <c:v>4552.0</c:v>
+                </c:pt>
+                <c:pt idx="4552">
+                  <c:v>4553.0</c:v>
+                </c:pt>
+                <c:pt idx="4553">
+                  <c:v>4554.0</c:v>
+                </c:pt>
+                <c:pt idx="4554">
+                  <c:v>4555.0</c:v>
+                </c:pt>
+                <c:pt idx="4555">
+                  <c:v>4556.0</c:v>
+                </c:pt>
+                <c:pt idx="4556">
+                  <c:v>4557.0</c:v>
+                </c:pt>
+                <c:pt idx="4557">
+                  <c:v>4558.0</c:v>
+                </c:pt>
+                <c:pt idx="4558">
+                  <c:v>4559.0</c:v>
+                </c:pt>
+                <c:pt idx="4559">
+                  <c:v>4560.0</c:v>
+                </c:pt>
+                <c:pt idx="4560">
+                  <c:v>4561.0</c:v>
+                </c:pt>
+                <c:pt idx="4561">
+                  <c:v>4562.0</c:v>
+                </c:pt>
+                <c:pt idx="4562">
+                  <c:v>4563.0</c:v>
+                </c:pt>
+                <c:pt idx="4563">
+                  <c:v>4564.0</c:v>
+                </c:pt>
+                <c:pt idx="4564">
+                  <c:v>4565.0</c:v>
+                </c:pt>
+                <c:pt idx="4565">
+                  <c:v>4566.0</c:v>
+                </c:pt>
+                <c:pt idx="4566">
+                  <c:v>4567.0</c:v>
+                </c:pt>
+                <c:pt idx="4567">
+                  <c:v>4568.0</c:v>
+                </c:pt>
+                <c:pt idx="4568">
+                  <c:v>4569.0</c:v>
+                </c:pt>
+                <c:pt idx="4569">
+                  <c:v>4570.0</c:v>
+                </c:pt>
+                <c:pt idx="4570">
+                  <c:v>4571.0</c:v>
+                </c:pt>
+                <c:pt idx="4571">
+                  <c:v>4572.0</c:v>
+                </c:pt>
+                <c:pt idx="4572">
+                  <c:v>4573.0</c:v>
+                </c:pt>
+                <c:pt idx="4573">
+                  <c:v>4574.0</c:v>
+                </c:pt>
+                <c:pt idx="4574">
+                  <c:v>4575.0</c:v>
+                </c:pt>
+                <c:pt idx="4575">
+                  <c:v>4576.0</c:v>
+                </c:pt>
+                <c:pt idx="4576">
+                  <c:v>4577.0</c:v>
+                </c:pt>
+                <c:pt idx="4577">
+                  <c:v>4578.0</c:v>
+                </c:pt>
+                <c:pt idx="4578">
+                  <c:v>4579.0</c:v>
+                </c:pt>
+                <c:pt idx="4579">
+                  <c:v>4580.0</c:v>
+                </c:pt>
+                <c:pt idx="4580">
+                  <c:v>4581.0</c:v>
+                </c:pt>
+                <c:pt idx="4581">
+                  <c:v>4582.0</c:v>
+                </c:pt>
+                <c:pt idx="4582">
+                  <c:v>4583.0</c:v>
+                </c:pt>
+                <c:pt idx="4583">
+                  <c:v>4584.0</c:v>
+                </c:pt>
+                <c:pt idx="4584">
+                  <c:v>4585.0</c:v>
+                </c:pt>
+                <c:pt idx="4585">
+                  <c:v>4586.0</c:v>
+                </c:pt>
+                <c:pt idx="4586">
+                  <c:v>4587.0</c:v>
+                </c:pt>
+                <c:pt idx="4587">
+                  <c:v>4588.0</c:v>
+                </c:pt>
+                <c:pt idx="4588">
+                  <c:v>4589.0</c:v>
+                </c:pt>
+                <c:pt idx="4589">
+                  <c:v>4590.0</c:v>
+                </c:pt>
+                <c:pt idx="4590">
+                  <c:v>4591.0</c:v>
+                </c:pt>
+                <c:pt idx="4591">
+                  <c:v>4592.0</c:v>
+                </c:pt>
+                <c:pt idx="4592">
+                  <c:v>4593.0</c:v>
+                </c:pt>
+                <c:pt idx="4593">
+                  <c:v>4594.0</c:v>
+                </c:pt>
+                <c:pt idx="4594">
+                  <c:v>4595.0</c:v>
+                </c:pt>
+                <c:pt idx="4595">
+                  <c:v>4596.0</c:v>
+                </c:pt>
+                <c:pt idx="4596">
+                  <c:v>4597.0</c:v>
+                </c:pt>
+                <c:pt idx="4597">
+                  <c:v>4598.0</c:v>
+                </c:pt>
+                <c:pt idx="4598">
+                  <c:v>4599.0</c:v>
+                </c:pt>
+                <c:pt idx="4599">
+                  <c:v>4600.0</c:v>
+                </c:pt>
+                <c:pt idx="4600">
+                  <c:v>4601.0</c:v>
+                </c:pt>
+                <c:pt idx="4601">
+                  <c:v>4602.0</c:v>
+                </c:pt>
+                <c:pt idx="4602">
+                  <c:v>4603.0</c:v>
+                </c:pt>
+                <c:pt idx="4603">
+                  <c:v>4604.0</c:v>
+                </c:pt>
+                <c:pt idx="4604">
+                  <c:v>4605.0</c:v>
+                </c:pt>
+                <c:pt idx="4605">
+                  <c:v>4606.0</c:v>
+                </c:pt>
+                <c:pt idx="4606">
+                  <c:v>4607.0</c:v>
+                </c:pt>
+                <c:pt idx="4607">
+                  <c:v>4608.0</c:v>
+                </c:pt>
+                <c:pt idx="4608">
+                  <c:v>4609.0</c:v>
+                </c:pt>
+                <c:pt idx="4609">
+                  <c:v>4610.0</c:v>
+                </c:pt>
+                <c:pt idx="4610">
+                  <c:v>4611.0</c:v>
+                </c:pt>
+                <c:pt idx="4611">
+                  <c:v>4612.0</c:v>
+                </c:pt>
+                <c:pt idx="4612">
+                  <c:v>4613.0</c:v>
+                </c:pt>
+                <c:pt idx="4613">
+                  <c:v>4614.0</c:v>
+                </c:pt>
+                <c:pt idx="4614">
+                  <c:v>4615.0</c:v>
+                </c:pt>
+                <c:pt idx="4615">
+                  <c:v>4616.0</c:v>
+                </c:pt>
+                <c:pt idx="4616">
+                  <c:v>4617.0</c:v>
+                </c:pt>
+                <c:pt idx="4617">
+                  <c:v>4618.0</c:v>
+                </c:pt>
+                <c:pt idx="4618">
+                  <c:v>4619.0</c:v>
+                </c:pt>
+                <c:pt idx="4619">
+                  <c:v>4620.0</c:v>
+                </c:pt>
+                <c:pt idx="4620">
+                  <c:v>4621.0</c:v>
+                </c:pt>
+                <c:pt idx="4621">
+                  <c:v>4622.0</c:v>
+                </c:pt>
+                <c:pt idx="4622">
+                  <c:v>4623.0</c:v>
+                </c:pt>
+                <c:pt idx="4623">
+                  <c:v>4624.0</c:v>
+                </c:pt>
+                <c:pt idx="4624">
+                  <c:v>4625.0</c:v>
+                </c:pt>
+                <c:pt idx="4625">
+                  <c:v>4626.0</c:v>
+                </c:pt>
+                <c:pt idx="4626">
+                  <c:v>4627.0</c:v>
+                </c:pt>
+                <c:pt idx="4627">
+                  <c:v>4628.0</c:v>
+                </c:pt>
+                <c:pt idx="4628">
+                  <c:v>4629.0</c:v>
+                </c:pt>
+                <c:pt idx="4629">
+                  <c:v>4630.0</c:v>
+                </c:pt>
+                <c:pt idx="4630">
+                  <c:v>4631.0</c:v>
+                </c:pt>
+                <c:pt idx="4631">
+                  <c:v>4632.0</c:v>
+                </c:pt>
+                <c:pt idx="4632">
+                  <c:v>4633.0</c:v>
+                </c:pt>
+                <c:pt idx="4633">
+                  <c:v>4634.0</c:v>
+                </c:pt>
+                <c:pt idx="4634">
+                  <c:v>4635.0</c:v>
+                </c:pt>
+                <c:pt idx="4635">
+                  <c:v>4636.0</c:v>
+                </c:pt>
+                <c:pt idx="4636">
+                  <c:v>4637.0</c:v>
+                </c:pt>
+                <c:pt idx="4637">
+                  <c:v>4638.0</c:v>
+                </c:pt>
+                <c:pt idx="4638">
+                  <c:v>4639.0</c:v>
+                </c:pt>
+                <c:pt idx="4639">
+                  <c:v>4640.0</c:v>
+                </c:pt>
+                <c:pt idx="4640">
+                  <c:v>4641.0</c:v>
+                </c:pt>
+                <c:pt idx="4641">
+                  <c:v>4642.0</c:v>
+                </c:pt>
+                <c:pt idx="4642">
+                  <c:v>4643.0</c:v>
+                </c:pt>
+                <c:pt idx="4643">
+                  <c:v>4644.0</c:v>
+                </c:pt>
+                <c:pt idx="4644">
+                  <c:v>4645.0</c:v>
+                </c:pt>
+                <c:pt idx="4645">
+                  <c:v>4646.0</c:v>
+                </c:pt>
+                <c:pt idx="4646">
+                  <c:v>4647.0</c:v>
+                </c:pt>
+                <c:pt idx="4647">
+                  <c:v>4648.0</c:v>
+                </c:pt>
+                <c:pt idx="4648">
+                  <c:v>4649.0</c:v>
+                </c:pt>
+                <c:pt idx="4649">
+                  <c:v>4650.0</c:v>
+                </c:pt>
+                <c:pt idx="4650">
+                  <c:v>4651.0</c:v>
+                </c:pt>
+                <c:pt idx="4651">
+                  <c:v>4652.0</c:v>
+                </c:pt>
+                <c:pt idx="4652">
+                  <c:v>4653.0</c:v>
+                </c:pt>
+                <c:pt idx="4653">
+                  <c:v>4654.0</c:v>
+                </c:pt>
+                <c:pt idx="4654">
+                  <c:v>4655.0</c:v>
+                </c:pt>
+                <c:pt idx="4655">
+                  <c:v>4656.0</c:v>
+                </c:pt>
+                <c:pt idx="4656">
+                  <c:v>4657.0</c:v>
+                </c:pt>
+                <c:pt idx="4657">
+                  <c:v>4658.0</c:v>
+                </c:pt>
+                <c:pt idx="4658">
+                  <c:v>4659.0</c:v>
+                </c:pt>
+                <c:pt idx="4659">
+                  <c:v>4660.0</c:v>
+                </c:pt>
+                <c:pt idx="4660">
+                  <c:v>4661.0</c:v>
+                </c:pt>
+                <c:pt idx="4661">
+                  <c:v>4662.0</c:v>
+                </c:pt>
+                <c:pt idx="4662">
+                  <c:v>4663.0</c:v>
+                </c:pt>
+                <c:pt idx="4663">
+                  <c:v>4664.0</c:v>
+                </c:pt>
+                <c:pt idx="4664">
+                  <c:v>4665.0</c:v>
+                </c:pt>
+                <c:pt idx="4665">
+                  <c:v>4666.0</c:v>
+                </c:pt>
+                <c:pt idx="4666">
+                  <c:v>4667.0</c:v>
+                </c:pt>
+                <c:pt idx="4667">
+                  <c:v>4668.0</c:v>
+                </c:pt>
+                <c:pt idx="4668">
+                  <c:v>4669.0</c:v>
+                </c:pt>
+                <c:pt idx="4669">
+                  <c:v>4670.0</c:v>
+                </c:pt>
+                <c:pt idx="4670">
+                  <c:v>4671.0</c:v>
+                </c:pt>
+                <c:pt idx="4671">
+                  <c:v>4672.0</c:v>
+                </c:pt>
+                <c:pt idx="4672">
+                  <c:v>4673.0</c:v>
+                </c:pt>
+                <c:pt idx="4673">
+                  <c:v>4674.0</c:v>
+                </c:pt>
+                <c:pt idx="4674">
+                  <c:v>4675.0</c:v>
+                </c:pt>
+                <c:pt idx="4675">
+                  <c:v>4676.0</c:v>
+                </c:pt>
+                <c:pt idx="4676">
+                  <c:v>4677.0</c:v>
+                </c:pt>
+                <c:pt idx="4677">
+                  <c:v>4678.0</c:v>
+                </c:pt>
+                <c:pt idx="4678">
+                  <c:v>4679.0</c:v>
+                </c:pt>
+                <c:pt idx="4679">
+                  <c:v>4680.0</c:v>
+                </c:pt>
+                <c:pt idx="4680">
+                  <c:v>4681.0</c:v>
+                </c:pt>
+                <c:pt idx="4681">
+                  <c:v>4682.0</c:v>
+                </c:pt>
+                <c:pt idx="4682">
+                  <c:v>4683.0</c:v>
+                </c:pt>
+                <c:pt idx="4683">
+                  <c:v>4684.0</c:v>
+                </c:pt>
+                <c:pt idx="4684">
+                  <c:v>4685.0</c:v>
+                </c:pt>
+                <c:pt idx="4685">
+                  <c:v>4686.0</c:v>
+                </c:pt>
+                <c:pt idx="4686">
+                  <c:v>4687.0</c:v>
+                </c:pt>
+                <c:pt idx="4687">
+                  <c:v>4688.0</c:v>
+                </c:pt>
+                <c:pt idx="4688">
+                  <c:v>4689.0</c:v>
+                </c:pt>
+                <c:pt idx="4689">
+                  <c:v>4690.0</c:v>
+                </c:pt>
+                <c:pt idx="4690">
+                  <c:v>4691.0</c:v>
+                </c:pt>
+                <c:pt idx="4691">
+                  <c:v>4692.0</c:v>
+                </c:pt>
+                <c:pt idx="4692">
+                  <c:v>4693.0</c:v>
+                </c:pt>
+                <c:pt idx="4693">
+                  <c:v>4694.0</c:v>
+                </c:pt>
+                <c:pt idx="4694">
+                  <c:v>4695.0</c:v>
+                </c:pt>
+                <c:pt idx="4695">
+                  <c:v>4696.0</c:v>
+                </c:pt>
+                <c:pt idx="4696">
+                  <c:v>4697.0</c:v>
+                </c:pt>
+                <c:pt idx="4697">
+                  <c:v>4698.0</c:v>
+                </c:pt>
+                <c:pt idx="4698">
+                  <c:v>4699.0</c:v>
+                </c:pt>
+                <c:pt idx="4699">
+                  <c:v>4700.0</c:v>
+                </c:pt>
+                <c:pt idx="4700">
+                  <c:v>4701.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -27310,34 +28384,33 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="2032232296"/>
-        <c:axId val="2032226696"/>
+        <c:axId val="-2108100600"/>
+        <c:axId val="-2108097592"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="2032232296"/>
+        <c:axId val="-2108100600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="41640.0"/>
-          <c:min val="39083.0"/>
+          <c:min val="39417.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="[$-409]mmmm\-yy;@" sourceLinked="0"/>
+        <c:numFmt formatCode="m/d/yy" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2032226696"/>
+        <c:crossAx val="-2108097592"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
-        <c:majorUnit val="6.0"/>
+        <c:majorUnit val="2.0"/>
         <c:majorTimeUnit val="months"/>
         <c:minorUnit val="1.0"/>
         <c:minorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2032226696"/>
+        <c:axId val="-2108097592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27348,7 +28421,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2032232296"/>
+        <c:crossAx val="-2108100600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -27841,6 +28914,9 @@
                 <c:pt idx="72">
                   <c:v>132.0</c:v>
                 </c:pt>
+                <c:pt idx="73">
+                  <c:v>208.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -27854,11 +28930,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="2106462648"/>
-        <c:axId val="2106465688"/>
+        <c:axId val="2122162024"/>
+        <c:axId val="2122165064"/>
       </c:barChart>
       <c:dateAx>
-        <c:axId val="2106462648"/>
+        <c:axId val="2122162024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27868,14 +28944,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106465688"/>
+        <c:crossAx val="2122165064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="2106465688"/>
+        <c:axId val="2122165064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -27886,7 +28962,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106462648"/>
+        <c:crossAx val="2122162024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -27902,10 +28978,9 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="141" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="133" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
 </chartsheet>
 </file>
@@ -27914,7 +28989,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="132" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -27926,10 +29001,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8565745" cy="5818582"/>
+    <xdr:ext cx="8574887" cy="5834361"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1" title="Data Packages in Dryad"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks noGrp="1"/>
         </xdr:cNvGraphicFramePr>
@@ -27953,7 +29028,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8565745" cy="5818582"/>
+    <xdr:ext cx="8572500" cy="5834063"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
@@ -27977,6 +29052,10 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="x" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="dryadSubmitDates" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
@@ -28302,10 +29381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4524"/>
+  <dimension ref="A1:B4701"/>
   <sheetViews>
-    <sheetView topLeftCell="A4465" workbookViewId="0">
-      <selection activeCell="A4493" sqref="A4493"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4701"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -64503,6 +65582,1422 @@
       </c>
       <c r="B4524">
         <v>4524</v>
+      </c>
+    </row>
+    <row r="4525" spans="1:2">
+      <c r="A4525" s="1">
+        <v>41645</v>
+      </c>
+      <c r="B4525">
+        <v>4525</v>
+      </c>
+    </row>
+    <row r="4526" spans="1:2">
+      <c r="A4526" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B4526">
+        <v>4526</v>
+      </c>
+    </row>
+    <row r="4527" spans="1:2">
+      <c r="A4527" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B4527">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="4528" spans="1:2">
+      <c r="A4528" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B4528">
+        <v>4528</v>
+      </c>
+    </row>
+    <row r="4529" spans="1:2">
+      <c r="A4529" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B4529">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="4530" spans="1:2">
+      <c r="A4530" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B4530">
+        <v>4530</v>
+      </c>
+    </row>
+    <row r="4531" spans="1:2">
+      <c r="A4531" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B4531">
+        <v>4531</v>
+      </c>
+    </row>
+    <row r="4532" spans="1:2">
+      <c r="A4532" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B4532">
+        <v>4532</v>
+      </c>
+    </row>
+    <row r="4533" spans="1:2">
+      <c r="A4533" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B4533">
+        <v>4533</v>
+      </c>
+    </row>
+    <row r="4534" spans="1:2">
+      <c r="A4534" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B4534">
+        <v>4534</v>
+      </c>
+    </row>
+    <row r="4535" spans="1:2">
+      <c r="A4535" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B4535">
+        <v>4535</v>
+      </c>
+    </row>
+    <row r="4536" spans="1:2">
+      <c r="A4536" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B4536">
+        <v>4536</v>
+      </c>
+    </row>
+    <row r="4537" spans="1:2">
+      <c r="A4537" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B4537">
+        <v>4537</v>
+      </c>
+    </row>
+    <row r="4538" spans="1:2">
+      <c r="A4538" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B4538">
+        <v>4538</v>
+      </c>
+    </row>
+    <row r="4539" spans="1:2">
+      <c r="A4539" s="1">
+        <v>41646</v>
+      </c>
+      <c r="B4539">
+        <v>4539</v>
+      </c>
+    </row>
+    <row r="4540" spans="1:2">
+      <c r="A4540" s="1">
+        <v>41647</v>
+      </c>
+      <c r="B4540">
+        <v>4540</v>
+      </c>
+    </row>
+    <row r="4541" spans="1:2">
+      <c r="A4541" s="1">
+        <v>41647</v>
+      </c>
+      <c r="B4541">
+        <v>4541</v>
+      </c>
+    </row>
+    <row r="4542" spans="1:2">
+      <c r="A4542" s="1">
+        <v>41647</v>
+      </c>
+      <c r="B4542">
+        <v>4542</v>
+      </c>
+    </row>
+    <row r="4543" spans="1:2">
+      <c r="A4543" s="1">
+        <v>41647</v>
+      </c>
+      <c r="B4543">
+        <v>4543</v>
+      </c>
+    </row>
+    <row r="4544" spans="1:2">
+      <c r="A4544" s="1">
+        <v>41647</v>
+      </c>
+      <c r="B4544">
+        <v>4544</v>
+      </c>
+    </row>
+    <row r="4545" spans="1:2">
+      <c r="A4545" s="1">
+        <v>41647</v>
+      </c>
+      <c r="B4545">
+        <v>4545</v>
+      </c>
+    </row>
+    <row r="4546" spans="1:2">
+      <c r="A4546" s="1">
+        <v>41647</v>
+      </c>
+      <c r="B4546">
+        <v>4546</v>
+      </c>
+    </row>
+    <row r="4547" spans="1:2">
+      <c r="A4547" s="1">
+        <v>41647</v>
+      </c>
+      <c r="B4547">
+        <v>4547</v>
+      </c>
+    </row>
+    <row r="4548" spans="1:2">
+      <c r="A4548" s="1">
+        <v>41647</v>
+      </c>
+      <c r="B4548">
+        <v>4548</v>
+      </c>
+    </row>
+    <row r="4549" spans="1:2">
+      <c r="A4549" s="1">
+        <v>41647</v>
+      </c>
+      <c r="B4549">
+        <v>4549</v>
+      </c>
+    </row>
+    <row r="4550" spans="1:2">
+      <c r="A4550" s="1">
+        <v>41648</v>
+      </c>
+      <c r="B4550">
+        <v>4550</v>
+      </c>
+    </row>
+    <row r="4551" spans="1:2">
+      <c r="A4551" s="1">
+        <v>41648</v>
+      </c>
+      <c r="B4551">
+        <v>4551</v>
+      </c>
+    </row>
+    <row r="4552" spans="1:2">
+      <c r="A4552" s="1">
+        <v>41648</v>
+      </c>
+      <c r="B4552">
+        <v>4552</v>
+      </c>
+    </row>
+    <row r="4553" spans="1:2">
+      <c r="A4553" s="1">
+        <v>41648</v>
+      </c>
+      <c r="B4553">
+        <v>4553</v>
+      </c>
+    </row>
+    <row r="4554" spans="1:2">
+      <c r="A4554" s="1">
+        <v>41648</v>
+      </c>
+      <c r="B4554">
+        <v>4554</v>
+      </c>
+    </row>
+    <row r="4555" spans="1:2">
+      <c r="A4555" s="1">
+        <v>41648</v>
+      </c>
+      <c r="B4555">
+        <v>4555</v>
+      </c>
+    </row>
+    <row r="4556" spans="1:2">
+      <c r="A4556" s="1">
+        <v>41648</v>
+      </c>
+      <c r="B4556">
+        <v>4556</v>
+      </c>
+    </row>
+    <row r="4557" spans="1:2">
+      <c r="A4557" s="1">
+        <v>41649</v>
+      </c>
+      <c r="B4557">
+        <v>4557</v>
+      </c>
+    </row>
+    <row r="4558" spans="1:2">
+      <c r="A4558" s="1">
+        <v>41649</v>
+      </c>
+      <c r="B4558">
+        <v>4558</v>
+      </c>
+    </row>
+    <row r="4559" spans="1:2">
+      <c r="A4559" s="1">
+        <v>41649</v>
+      </c>
+      <c r="B4559">
+        <v>4559</v>
+      </c>
+    </row>
+    <row r="4560" spans="1:2">
+      <c r="A4560" s="1">
+        <v>41649</v>
+      </c>
+      <c r="B4560">
+        <v>4560</v>
+      </c>
+    </row>
+    <row r="4561" spans="1:2">
+      <c r="A4561" s="1">
+        <v>41649</v>
+      </c>
+      <c r="B4561">
+        <v>4561</v>
+      </c>
+    </row>
+    <row r="4562" spans="1:2">
+      <c r="A4562" s="1">
+        <v>41649</v>
+      </c>
+      <c r="B4562">
+        <v>4562</v>
+      </c>
+    </row>
+    <row r="4563" spans="1:2">
+      <c r="A4563" s="1">
+        <v>41649</v>
+      </c>
+      <c r="B4563">
+        <v>4563</v>
+      </c>
+    </row>
+    <row r="4564" spans="1:2">
+      <c r="A4564" s="1">
+        <v>41652</v>
+      </c>
+      <c r="B4564">
+        <v>4564</v>
+      </c>
+    </row>
+    <row r="4565" spans="1:2">
+      <c r="A4565" s="1">
+        <v>41652</v>
+      </c>
+      <c r="B4565">
+        <v>4565</v>
+      </c>
+    </row>
+    <row r="4566" spans="1:2">
+      <c r="A4566" s="1">
+        <v>41652</v>
+      </c>
+      <c r="B4566">
+        <v>4566</v>
+      </c>
+    </row>
+    <row r="4567" spans="1:2">
+      <c r="A4567" s="1">
+        <v>41652</v>
+      </c>
+      <c r="B4567">
+        <v>4567</v>
+      </c>
+    </row>
+    <row r="4568" spans="1:2">
+      <c r="A4568" s="1">
+        <v>41652</v>
+      </c>
+      <c r="B4568">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="4569" spans="1:2">
+      <c r="A4569" s="1">
+        <v>41653</v>
+      </c>
+      <c r="B4569">
+        <v>4569</v>
+      </c>
+    </row>
+    <row r="4570" spans="1:2">
+      <c r="A4570" s="1">
+        <v>41653</v>
+      </c>
+      <c r="B4570">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="4571" spans="1:2">
+      <c r="A4571" s="1">
+        <v>41653</v>
+      </c>
+      <c r="B4571">
+        <v>4571</v>
+      </c>
+    </row>
+    <row r="4572" spans="1:2">
+      <c r="A4572" s="1">
+        <v>41653</v>
+      </c>
+      <c r="B4572">
+        <v>4572</v>
+      </c>
+    </row>
+    <row r="4573" spans="1:2">
+      <c r="A4573" s="1">
+        <v>41653</v>
+      </c>
+      <c r="B4573">
+        <v>4573</v>
+      </c>
+    </row>
+    <row r="4574" spans="1:2">
+      <c r="A4574" s="1">
+        <v>41653</v>
+      </c>
+      <c r="B4574">
+        <v>4574</v>
+      </c>
+    </row>
+    <row r="4575" spans="1:2">
+      <c r="A4575" s="1">
+        <v>41653</v>
+      </c>
+      <c r="B4575">
+        <v>4575</v>
+      </c>
+    </row>
+    <row r="4576" spans="1:2">
+      <c r="A4576" s="1">
+        <v>41653</v>
+      </c>
+      <c r="B4576">
+        <v>4576</v>
+      </c>
+    </row>
+    <row r="4577" spans="1:2">
+      <c r="A4577" s="1">
+        <v>41653</v>
+      </c>
+      <c r="B4577">
+        <v>4577</v>
+      </c>
+    </row>
+    <row r="4578" spans="1:2">
+      <c r="A4578" s="1">
+        <v>41653</v>
+      </c>
+      <c r="B4578">
+        <v>4578</v>
+      </c>
+    </row>
+    <row r="4579" spans="1:2">
+      <c r="A4579" s="1">
+        <v>41653</v>
+      </c>
+      <c r="B4579">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="4580" spans="1:2">
+      <c r="A4580" s="1">
+        <v>41653</v>
+      </c>
+      <c r="B4580">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="4581" spans="1:2">
+      <c r="A4581" s="1">
+        <v>41653</v>
+      </c>
+      <c r="B4581">
+        <v>4581</v>
+      </c>
+    </row>
+    <row r="4582" spans="1:2">
+      <c r="A4582" s="1">
+        <v>41653</v>
+      </c>
+      <c r="B4582">
+        <v>4582</v>
+      </c>
+    </row>
+    <row r="4583" spans="1:2">
+      <c r="A4583" s="1">
+        <v>41653</v>
+      </c>
+      <c r="B4583">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="4584" spans="1:2">
+      <c r="A4584" s="1">
+        <v>41653</v>
+      </c>
+      <c r="B4584">
+        <v>4584</v>
+      </c>
+    </row>
+    <row r="4585" spans="1:2">
+      <c r="A4585" s="1">
+        <v>41653</v>
+      </c>
+      <c r="B4585">
+        <v>4585</v>
+      </c>
+    </row>
+    <row r="4586" spans="1:2">
+      <c r="A4586" s="1">
+        <v>41653</v>
+      </c>
+      <c r="B4586">
+        <v>4586</v>
+      </c>
+    </row>
+    <row r="4587" spans="1:2">
+      <c r="A4587" s="1">
+        <v>41654</v>
+      </c>
+      <c r="B4587">
+        <v>4587</v>
+      </c>
+    </row>
+    <row r="4588" spans="1:2">
+      <c r="A4588" s="1">
+        <v>41654</v>
+      </c>
+      <c r="B4588">
+        <v>4588</v>
+      </c>
+    </row>
+    <row r="4589" spans="1:2">
+      <c r="A4589" s="1">
+        <v>41654</v>
+      </c>
+      <c r="B4589">
+        <v>4589</v>
+      </c>
+    </row>
+    <row r="4590" spans="1:2">
+      <c r="A4590" s="1">
+        <v>41654</v>
+      </c>
+      <c r="B4590">
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="4591" spans="1:2">
+      <c r="A4591" s="1">
+        <v>41654</v>
+      </c>
+      <c r="B4591">
+        <v>4591</v>
+      </c>
+    </row>
+    <row r="4592" spans="1:2">
+      <c r="A4592" s="1">
+        <v>41654</v>
+      </c>
+      <c r="B4592">
+        <v>4592</v>
+      </c>
+    </row>
+    <row r="4593" spans="1:2">
+      <c r="A4593" s="1">
+        <v>41654</v>
+      </c>
+      <c r="B4593">
+        <v>4593</v>
+      </c>
+    </row>
+    <row r="4594" spans="1:2">
+      <c r="A4594" s="1">
+        <v>41654</v>
+      </c>
+      <c r="B4594">
+        <v>4594</v>
+      </c>
+    </row>
+    <row r="4595" spans="1:2">
+      <c r="A4595" s="1">
+        <v>41654</v>
+      </c>
+      <c r="B4595">
+        <v>4595</v>
+      </c>
+    </row>
+    <row r="4596" spans="1:2">
+      <c r="A4596" s="1">
+        <v>41654</v>
+      </c>
+      <c r="B4596">
+        <v>4596</v>
+      </c>
+    </row>
+    <row r="4597" spans="1:2">
+      <c r="A4597" s="1">
+        <v>41654</v>
+      </c>
+      <c r="B4597">
+        <v>4597</v>
+      </c>
+    </row>
+    <row r="4598" spans="1:2">
+      <c r="A4598" s="1">
+        <v>41654</v>
+      </c>
+      <c r="B4598">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="4599" spans="1:2">
+      <c r="A4599" s="1">
+        <v>41654</v>
+      </c>
+      <c r="B4599">
+        <v>4599</v>
+      </c>
+    </row>
+    <row r="4600" spans="1:2">
+      <c r="A4600" s="1">
+        <v>41655</v>
+      </c>
+      <c r="B4600">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="4601" spans="1:2">
+      <c r="A4601" s="1">
+        <v>41655</v>
+      </c>
+      <c r="B4601">
+        <v>4601</v>
+      </c>
+    </row>
+    <row r="4602" spans="1:2">
+      <c r="A4602" s="1">
+        <v>41655</v>
+      </c>
+      <c r="B4602">
+        <v>4602</v>
+      </c>
+    </row>
+    <row r="4603" spans="1:2">
+      <c r="A4603" s="1">
+        <v>41655</v>
+      </c>
+      <c r="B4603">
+        <v>4603</v>
+      </c>
+    </row>
+    <row r="4604" spans="1:2">
+      <c r="A4604" s="1">
+        <v>41656</v>
+      </c>
+      <c r="B4604">
+        <v>4604</v>
+      </c>
+    </row>
+    <row r="4605" spans="1:2">
+      <c r="A4605" s="1">
+        <v>41656</v>
+      </c>
+      <c r="B4605">
+        <v>4605</v>
+      </c>
+    </row>
+    <row r="4606" spans="1:2">
+      <c r="A4606" s="1">
+        <v>41656</v>
+      </c>
+      <c r="B4606">
+        <v>4606</v>
+      </c>
+    </row>
+    <row r="4607" spans="1:2">
+      <c r="A4607" s="1">
+        <v>41656</v>
+      </c>
+      <c r="B4607">
+        <v>4607</v>
+      </c>
+    </row>
+    <row r="4608" spans="1:2">
+      <c r="A4608" s="1">
+        <v>41660</v>
+      </c>
+      <c r="B4608">
+        <v>4608</v>
+      </c>
+    </row>
+    <row r="4609" spans="1:2">
+      <c r="A4609" s="1">
+        <v>41660</v>
+      </c>
+      <c r="B4609">
+        <v>4609</v>
+      </c>
+    </row>
+    <row r="4610" spans="1:2">
+      <c r="A4610" s="1">
+        <v>41660</v>
+      </c>
+      <c r="B4610">
+        <v>4610</v>
+      </c>
+    </row>
+    <row r="4611" spans="1:2">
+      <c r="A4611" s="1">
+        <v>41660</v>
+      </c>
+      <c r="B4611">
+        <v>4611</v>
+      </c>
+    </row>
+    <row r="4612" spans="1:2">
+      <c r="A4612" s="1">
+        <v>41660</v>
+      </c>
+      <c r="B4612">
+        <v>4612</v>
+      </c>
+    </row>
+    <row r="4613" spans="1:2">
+      <c r="A4613" s="1">
+        <v>41660</v>
+      </c>
+      <c r="B4613">
+        <v>4613</v>
+      </c>
+    </row>
+    <row r="4614" spans="1:2">
+      <c r="A4614" s="1">
+        <v>41660</v>
+      </c>
+      <c r="B4614">
+        <v>4614</v>
+      </c>
+    </row>
+    <row r="4615" spans="1:2">
+      <c r="A4615" s="1">
+        <v>41660</v>
+      </c>
+      <c r="B4615">
+        <v>4615</v>
+      </c>
+    </row>
+    <row r="4616" spans="1:2">
+      <c r="A4616" s="1">
+        <v>41660</v>
+      </c>
+      <c r="B4616">
+        <v>4616</v>
+      </c>
+    </row>
+    <row r="4617" spans="1:2">
+      <c r="A4617" s="1">
+        <v>41660</v>
+      </c>
+      <c r="B4617">
+        <v>4617</v>
+      </c>
+    </row>
+    <row r="4618" spans="1:2">
+      <c r="A4618" s="1">
+        <v>41660</v>
+      </c>
+      <c r="B4618">
+        <v>4618</v>
+      </c>
+    </row>
+    <row r="4619" spans="1:2">
+      <c r="A4619" s="1">
+        <v>41660</v>
+      </c>
+      <c r="B4619">
+        <v>4619</v>
+      </c>
+    </row>
+    <row r="4620" spans="1:2">
+      <c r="A4620" s="1">
+        <v>41660</v>
+      </c>
+      <c r="B4620">
+        <v>4620</v>
+      </c>
+    </row>
+    <row r="4621" spans="1:2">
+      <c r="A4621" s="1">
+        <v>41660</v>
+      </c>
+      <c r="B4621">
+        <v>4621</v>
+      </c>
+    </row>
+    <row r="4622" spans="1:2">
+      <c r="A4622" s="1">
+        <v>41660</v>
+      </c>
+      <c r="B4622">
+        <v>4622</v>
+      </c>
+    </row>
+    <row r="4623" spans="1:2">
+      <c r="A4623" s="1">
+        <v>41660</v>
+      </c>
+      <c r="B4623">
+        <v>4623</v>
+      </c>
+    </row>
+    <row r="4624" spans="1:2">
+      <c r="A4624" s="1">
+        <v>41660</v>
+      </c>
+      <c r="B4624">
+        <v>4624</v>
+      </c>
+    </row>
+    <row r="4625" spans="1:2">
+      <c r="A4625" s="1">
+        <v>41660</v>
+      </c>
+      <c r="B4625">
+        <v>4625</v>
+      </c>
+    </row>
+    <row r="4626" spans="1:2">
+      <c r="A4626" s="1">
+        <v>41660</v>
+      </c>
+      <c r="B4626">
+        <v>4626</v>
+      </c>
+    </row>
+    <row r="4627" spans="1:2">
+      <c r="A4627" s="1">
+        <v>41660</v>
+      </c>
+      <c r="B4627">
+        <v>4627</v>
+      </c>
+    </row>
+    <row r="4628" spans="1:2">
+      <c r="A4628" s="1">
+        <v>41661</v>
+      </c>
+      <c r="B4628">
+        <v>4628</v>
+      </c>
+    </row>
+    <row r="4629" spans="1:2">
+      <c r="A4629" s="1">
+        <v>41661</v>
+      </c>
+      <c r="B4629">
+        <v>4629</v>
+      </c>
+    </row>
+    <row r="4630" spans="1:2">
+      <c r="A4630" s="1">
+        <v>41661</v>
+      </c>
+      <c r="B4630">
+        <v>4630</v>
+      </c>
+    </row>
+    <row r="4631" spans="1:2">
+      <c r="A4631" s="1">
+        <v>41661</v>
+      </c>
+      <c r="B4631">
+        <v>4631</v>
+      </c>
+    </row>
+    <row r="4632" spans="1:2">
+      <c r="A4632" s="1">
+        <v>41661</v>
+      </c>
+      <c r="B4632">
+        <v>4632</v>
+      </c>
+    </row>
+    <row r="4633" spans="1:2">
+      <c r="A4633" s="1">
+        <v>41661</v>
+      </c>
+      <c r="B4633">
+        <v>4633</v>
+      </c>
+    </row>
+    <row r="4634" spans="1:2">
+      <c r="A4634" s="1">
+        <v>41661</v>
+      </c>
+      <c r="B4634">
+        <v>4634</v>
+      </c>
+    </row>
+    <row r="4635" spans="1:2">
+      <c r="A4635" s="1">
+        <v>41661</v>
+      </c>
+      <c r="B4635">
+        <v>4635</v>
+      </c>
+    </row>
+    <row r="4636" spans="1:2">
+      <c r="A4636" s="1">
+        <v>41661</v>
+      </c>
+      <c r="B4636">
+        <v>4636</v>
+      </c>
+    </row>
+    <row r="4637" spans="1:2">
+      <c r="A4637" s="1">
+        <v>41661</v>
+      </c>
+      <c r="B4637">
+        <v>4637</v>
+      </c>
+    </row>
+    <row r="4638" spans="1:2">
+      <c r="A4638" s="1">
+        <v>41661</v>
+      </c>
+      <c r="B4638">
+        <v>4638</v>
+      </c>
+    </row>
+    <row r="4639" spans="1:2">
+      <c r="A4639" s="1">
+        <v>41661</v>
+      </c>
+      <c r="B4639">
+        <v>4639</v>
+      </c>
+    </row>
+    <row r="4640" spans="1:2">
+      <c r="A4640" s="1">
+        <v>41661</v>
+      </c>
+      <c r="B4640">
+        <v>4640</v>
+      </c>
+    </row>
+    <row r="4641" spans="1:2">
+      <c r="A4641" s="1">
+        <v>41662</v>
+      </c>
+      <c r="B4641">
+        <v>4641</v>
+      </c>
+    </row>
+    <row r="4642" spans="1:2">
+      <c r="A4642" s="1">
+        <v>41662</v>
+      </c>
+      <c r="B4642">
+        <v>4642</v>
+      </c>
+    </row>
+    <row r="4643" spans="1:2">
+      <c r="A4643" s="1">
+        <v>41662</v>
+      </c>
+      <c r="B4643">
+        <v>4643</v>
+      </c>
+    </row>
+    <row r="4644" spans="1:2">
+      <c r="A4644" s="1">
+        <v>41662</v>
+      </c>
+      <c r="B4644">
+        <v>4644</v>
+      </c>
+    </row>
+    <row r="4645" spans="1:2">
+      <c r="A4645" s="1">
+        <v>41662</v>
+      </c>
+      <c r="B4645">
+        <v>4645</v>
+      </c>
+    </row>
+    <row r="4646" spans="1:2">
+      <c r="A4646" s="1">
+        <v>41662</v>
+      </c>
+      <c r="B4646">
+        <v>4646</v>
+      </c>
+    </row>
+    <row r="4647" spans="1:2">
+      <c r="A4647" s="1">
+        <v>41663</v>
+      </c>
+      <c r="B4647">
+        <v>4647</v>
+      </c>
+    </row>
+    <row r="4648" spans="1:2">
+      <c r="A4648" s="1">
+        <v>41663</v>
+      </c>
+      <c r="B4648">
+        <v>4648</v>
+      </c>
+    </row>
+    <row r="4649" spans="1:2">
+      <c r="A4649" s="1">
+        <v>41663</v>
+      </c>
+      <c r="B4649">
+        <v>4649</v>
+      </c>
+    </row>
+    <row r="4650" spans="1:2">
+      <c r="A4650" s="1">
+        <v>41663</v>
+      </c>
+      <c r="B4650">
+        <v>4650</v>
+      </c>
+    </row>
+    <row r="4651" spans="1:2">
+      <c r="A4651" s="1">
+        <v>41666</v>
+      </c>
+      <c r="B4651">
+        <v>4651</v>
+      </c>
+    </row>
+    <row r="4652" spans="1:2">
+      <c r="A4652" s="1">
+        <v>41666</v>
+      </c>
+      <c r="B4652">
+        <v>4652</v>
+      </c>
+    </row>
+    <row r="4653" spans="1:2">
+      <c r="A4653" s="1">
+        <v>41666</v>
+      </c>
+      <c r="B4653">
+        <v>4653</v>
+      </c>
+    </row>
+    <row r="4654" spans="1:2">
+      <c r="A4654" s="1">
+        <v>41666</v>
+      </c>
+      <c r="B4654">
+        <v>4654</v>
+      </c>
+    </row>
+    <row r="4655" spans="1:2">
+      <c r="A4655" s="1">
+        <v>41666</v>
+      </c>
+      <c r="B4655">
+        <v>4655</v>
+      </c>
+    </row>
+    <row r="4656" spans="1:2">
+      <c r="A4656" s="1">
+        <v>41666</v>
+      </c>
+      <c r="B4656">
+        <v>4656</v>
+      </c>
+    </row>
+    <row r="4657" spans="1:2">
+      <c r="A4657" s="1">
+        <v>41666</v>
+      </c>
+      <c r="B4657">
+        <v>4657</v>
+      </c>
+    </row>
+    <row r="4658" spans="1:2">
+      <c r="A4658" s="1">
+        <v>41666</v>
+      </c>
+      <c r="B4658">
+        <v>4658</v>
+      </c>
+    </row>
+    <row r="4659" spans="1:2">
+      <c r="A4659" s="1">
+        <v>41666</v>
+      </c>
+      <c r="B4659">
+        <v>4659</v>
+      </c>
+    </row>
+    <row r="4660" spans="1:2">
+      <c r="A4660" s="1">
+        <v>41666</v>
+      </c>
+      <c r="B4660">
+        <v>4660</v>
+      </c>
+    </row>
+    <row r="4661" spans="1:2">
+      <c r="A4661" s="1">
+        <v>41666</v>
+      </c>
+      <c r="B4661">
+        <v>4661</v>
+      </c>
+    </row>
+    <row r="4662" spans="1:2">
+      <c r="A4662" s="1">
+        <v>41666</v>
+      </c>
+      <c r="B4662">
+        <v>4662</v>
+      </c>
+    </row>
+    <row r="4663" spans="1:2">
+      <c r="A4663" s="1">
+        <v>41666</v>
+      </c>
+      <c r="B4663">
+        <v>4663</v>
+      </c>
+    </row>
+    <row r="4664" spans="1:2">
+      <c r="A4664" s="1">
+        <v>41666</v>
+      </c>
+      <c r="B4664">
+        <v>4664</v>
+      </c>
+    </row>
+    <row r="4665" spans="1:2">
+      <c r="A4665" s="1">
+        <v>41666</v>
+      </c>
+      <c r="B4665">
+        <v>4665</v>
+      </c>
+    </row>
+    <row r="4666" spans="1:2">
+      <c r="A4666" s="1">
+        <v>41666</v>
+      </c>
+      <c r="B4666">
+        <v>4666</v>
+      </c>
+    </row>
+    <row r="4667" spans="1:2">
+      <c r="A4667" s="1">
+        <v>41666</v>
+      </c>
+      <c r="B4667">
+        <v>4667</v>
+      </c>
+    </row>
+    <row r="4668" spans="1:2">
+      <c r="A4668" s="1">
+        <v>41666</v>
+      </c>
+      <c r="B4668">
+        <v>4668</v>
+      </c>
+    </row>
+    <row r="4669" spans="1:2">
+      <c r="A4669" s="1">
+        <v>41666</v>
+      </c>
+      <c r="B4669">
+        <v>4669</v>
+      </c>
+    </row>
+    <row r="4670" spans="1:2">
+      <c r="A4670" s="1">
+        <v>41666</v>
+      </c>
+      <c r="B4670">
+        <v>4670</v>
+      </c>
+    </row>
+    <row r="4671" spans="1:2">
+      <c r="A4671" s="1">
+        <v>41667</v>
+      </c>
+      <c r="B4671">
+        <v>4671</v>
+      </c>
+    </row>
+    <row r="4672" spans="1:2">
+      <c r="A4672" s="1">
+        <v>41667</v>
+      </c>
+      <c r="B4672">
+        <v>4672</v>
+      </c>
+    </row>
+    <row r="4673" spans="1:2">
+      <c r="A4673" s="1">
+        <v>41667</v>
+      </c>
+      <c r="B4673">
+        <v>4673</v>
+      </c>
+    </row>
+    <row r="4674" spans="1:2">
+      <c r="A4674" s="1">
+        <v>41667</v>
+      </c>
+      <c r="B4674">
+        <v>4674</v>
+      </c>
+    </row>
+    <row r="4675" spans="1:2">
+      <c r="A4675" s="1">
+        <v>41667</v>
+      </c>
+      <c r="B4675">
+        <v>4675</v>
+      </c>
+    </row>
+    <row r="4676" spans="1:2">
+      <c r="A4676" s="1">
+        <v>41667</v>
+      </c>
+      <c r="B4676">
+        <v>4676</v>
+      </c>
+    </row>
+    <row r="4677" spans="1:2">
+      <c r="A4677" s="1">
+        <v>41667</v>
+      </c>
+      <c r="B4677">
+        <v>4677</v>
+      </c>
+    </row>
+    <row r="4678" spans="1:2">
+      <c r="A4678" s="1">
+        <v>41667</v>
+      </c>
+      <c r="B4678">
+        <v>4678</v>
+      </c>
+    </row>
+    <row r="4679" spans="1:2">
+      <c r="A4679" s="1">
+        <v>41667</v>
+      </c>
+      <c r="B4679">
+        <v>4679</v>
+      </c>
+    </row>
+    <row r="4680" spans="1:2">
+      <c r="A4680" s="1">
+        <v>41667</v>
+      </c>
+      <c r="B4680">
+        <v>4680</v>
+      </c>
+    </row>
+    <row r="4681" spans="1:2">
+      <c r="A4681" s="1">
+        <v>41667</v>
+      </c>
+      <c r="B4681">
+        <v>4681</v>
+      </c>
+    </row>
+    <row r="4682" spans="1:2">
+      <c r="A4682" s="1">
+        <v>41668</v>
+      </c>
+      <c r="B4682">
+        <v>4682</v>
+      </c>
+    </row>
+    <row r="4683" spans="1:2">
+      <c r="A4683" s="1">
+        <v>41668</v>
+      </c>
+      <c r="B4683">
+        <v>4683</v>
+      </c>
+    </row>
+    <row r="4684" spans="1:2">
+      <c r="A4684" s="1">
+        <v>41668</v>
+      </c>
+      <c r="B4684">
+        <v>4684</v>
+      </c>
+    </row>
+    <row r="4685" spans="1:2">
+      <c r="A4685" s="1">
+        <v>41668</v>
+      </c>
+      <c r="B4685">
+        <v>4685</v>
+      </c>
+    </row>
+    <row r="4686" spans="1:2">
+      <c r="A4686" s="1">
+        <v>41668</v>
+      </c>
+      <c r="B4686">
+        <v>4686</v>
+      </c>
+    </row>
+    <row r="4687" spans="1:2">
+      <c r="A4687" s="1">
+        <v>41668</v>
+      </c>
+      <c r="B4687">
+        <v>4687</v>
+      </c>
+    </row>
+    <row r="4688" spans="1:2">
+      <c r="A4688" s="1">
+        <v>41668</v>
+      </c>
+      <c r="B4688">
+        <v>4688</v>
+      </c>
+    </row>
+    <row r="4689" spans="1:2">
+      <c r="A4689" s="1">
+        <v>41668</v>
+      </c>
+      <c r="B4689">
+        <v>4689</v>
+      </c>
+    </row>
+    <row r="4690" spans="1:2">
+      <c r="A4690" s="1">
+        <v>41668</v>
+      </c>
+      <c r="B4690">
+        <v>4690</v>
+      </c>
+    </row>
+    <row r="4691" spans="1:2">
+      <c r="A4691" s="1">
+        <v>41668</v>
+      </c>
+      <c r="B4691">
+        <v>4691</v>
+      </c>
+    </row>
+    <row r="4692" spans="1:2">
+      <c r="A4692" s="1">
+        <v>41668</v>
+      </c>
+      <c r="B4692">
+        <v>4692</v>
+      </c>
+    </row>
+    <row r="4693" spans="1:2">
+      <c r="A4693" s="1">
+        <v>41669</v>
+      </c>
+      <c r="B4693">
+        <v>4693</v>
+      </c>
+    </row>
+    <row r="4694" spans="1:2">
+      <c r="A4694" s="1">
+        <v>41669</v>
+      </c>
+      <c r="B4694">
+        <v>4694</v>
+      </c>
+    </row>
+    <row r="4695" spans="1:2">
+      <c r="A4695" s="1">
+        <v>41669</v>
+      </c>
+      <c r="B4695">
+        <v>4695</v>
+      </c>
+    </row>
+    <row r="4696" spans="1:2">
+      <c r="A4696" s="1">
+        <v>41669</v>
+      </c>
+      <c r="B4696">
+        <v>4696</v>
+      </c>
+    </row>
+    <row r="4697" spans="1:2">
+      <c r="A4697" s="1">
+        <v>41669</v>
+      </c>
+      <c r="B4697">
+        <v>4697</v>
+      </c>
+    </row>
+    <row r="4698" spans="1:2">
+      <c r="A4698" s="1">
+        <v>41670</v>
+      </c>
+      <c r="B4698">
+        <v>4698</v>
+      </c>
+    </row>
+    <row r="4699" spans="1:2">
+      <c r="A4699" s="1">
+        <v>41670</v>
+      </c>
+      <c r="B4699">
+        <v>4699</v>
+      </c>
+    </row>
+    <row r="4700" spans="1:2">
+      <c r="A4700" s="1">
+        <v>41670</v>
+      </c>
+      <c r="B4700">
+        <v>4700</v>
+      </c>
+    </row>
+    <row r="4701" spans="1:2">
+      <c r="A4701" s="1">
+        <v>41670</v>
+      </c>
+      <c r="B4701">
+        <v>4701</v>
       </c>
     </row>
   </sheetData>
@@ -64521,9 +67016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B74"/>
   <sheetViews>
-    <sheetView topLeftCell="A45" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
@@ -65114,6 +67607,9 @@
     <row r="74" spans="1:2">
       <c r="A74" s="1">
         <v>41640</v>
+      </c>
+      <c r="B74">
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>